<commit_message>
updating lat_arb to lat_carb
</commit_message>
<xml_diff>
--- a/feedback_forms/current_versions/landfill_operator_feedback_v070.xlsx
+++ b/feedback_forms/current_versions/landfill_operator_feedback_v070.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\one_drive\code\pycharm\feedback_portal\feedback_forms\current_versions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carb-my.sharepoint.com/personal/tony_held_arb_ca_gov/Documents/code/pycharm/feedback_portal/feedback_forms/current_versions/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1058FBB9-DD57-4A6E-B0E3-E8E723D41AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5007" yWindow="2733" windowWidth="17413" windowHeight="11467" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
+    <workbookView xWindow="-25110" yWindow="1635" windowWidth="24195" windowHeight="11655" tabRatio="705" activeTab="5" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="6" r:id="rId1"/>
@@ -3815,21 +3815,21 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:AG73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.1171875" style="19" customWidth="1"/>
-    <col min="2" max="2" width="65.703125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="4.703125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="65.703125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="4.1171875" style="19" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="65.7109375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="65.7109375" style="19" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" style="19" customWidth="1"/>
     <col min="6" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
@@ -3865,7 +3865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:33" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:33" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="B2" s="31" t="s">
         <v>1</v>
       </c>
@@ -3874,7 +3874,7 @@
       <c r="E2" s="31"/>
       <c r="F2" s="49"/>
     </row>
-    <row r="3" spans="2:33" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:33" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
@@ -3883,13 +3883,13 @@
       <c r="E3" s="31"/>
       <c r="F3" s="50"/>
     </row>
-    <row r="4" spans="2:33" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:33" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="32"/>
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
       <c r="E4" s="33"/>
     </row>
-    <row r="5" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
       <c r="D6" s="51"/>
@@ -3959,12 +3959,12 @@
       <c r="AF6" s="52"/>
       <c r="AG6" s="52"/>
     </row>
-    <row r="7" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG7" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="75" t="s">
         <v>389</v>
       </c>
@@ -3973,7 +3973,7 @@
       <c r="E8" s="35"/>
       <c r="F8" s="49"/>
     </row>
-    <row r="9" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="62" t="s">
         <v>284</v>
       </c>
@@ -3982,7 +3982,7 @@
       <c r="E9" s="35"/>
       <c r="F9" s="49"/>
     </row>
-    <row r="10" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="63" t="s">
         <v>285</v>
       </c>
@@ -3991,7 +3991,7 @@
       <c r="E10" s="35"/>
       <c r="F10" s="49"/>
     </row>
-    <row r="11" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="64" t="s">
         <v>286</v>
       </c>
@@ -4000,7 +4000,7 @@
       <c r="E11" s="35"/>
       <c r="F11" s="49"/>
     </row>
-    <row r="12" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="61" t="s">
         <v>282</v>
       </c>
@@ -4009,7 +4009,7 @@
       <c r="E12" s="35"/>
       <c r="F12" s="49"/>
     </row>
-    <row r="13" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="61" t="s">
         <v>283</v>
       </c>
@@ -4018,7 +4018,7 @@
       <c r="E13" s="35"/>
       <c r="F13" s="49"/>
     </row>
-    <row r="14" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="75" t="s">
         <v>390</v>
       </c>
@@ -4027,7 +4027,7 @@
       <c r="E14" s="35"/>
       <c r="F14" s="49"/>
     </row>
-    <row r="15" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="75" t="s">
         <v>391</v>
       </c>
@@ -4036,7 +4036,7 @@
       <c r="E15" s="35"/>
       <c r="F15" s="49"/>
     </row>
-    <row r="16" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="61" t="s">
         <v>287</v>
       </c>
@@ -4045,7 +4045,7 @@
       <c r="E16" s="35"/>
       <c r="F16" s="49"/>
     </row>
-    <row r="17" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="75" t="s">
         <v>392</v>
       </c>
@@ -4054,7 +4054,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="49"/>
     </row>
-    <row r="18" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="65" t="s">
         <v>288</v>
       </c>
@@ -4063,12 +4063,12 @@
       <c r="E18" s="35"/>
       <c r="F18" s="49"/>
     </row>
-    <row r="20" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG20" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="51"/>
@@ -4102,12 +4102,12 @@
       <c r="AF21" s="52"/>
       <c r="AG21" s="52"/>
     </row>
-    <row r="22" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG22" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="74" t="s">
         <v>371</v>
       </c>
@@ -4118,7 +4118,7 @@
       <c r="E23" s="48"/>
       <c r="G23" s="36"/>
     </row>
-    <row r="24" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="74" t="s">
         <v>372</v>
       </c>
@@ -4128,7 +4128,7 @@
       </c>
       <c r="E24" s="35"/>
     </row>
-    <row r="25" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="74" t="s">
         <v>373</v>
       </c>
@@ -4138,7 +4138,7 @@
       </c>
       <c r="E25" s="35"/>
     </row>
-    <row r="26" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="75" t="s">
         <v>395</v>
       </c>
@@ -4149,7 +4149,7 @@
       <c r="E26" s="48"/>
       <c r="G26" s="36"/>
     </row>
-    <row r="27" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="74" t="s">
         <v>374</v>
       </c>
@@ -4160,7 +4160,7 @@
       <c r="E27" s="48"/>
       <c r="G27" s="36"/>
     </row>
-    <row r="28" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="76" t="s">
         <v>396</v>
       </c>
@@ -4172,12 +4172,12 @@
       <c r="F28" s="49"/>
       <c r="G28" s="36"/>
     </row>
-    <row r="29" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG29" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
       <c r="D30" s="51"/>
@@ -4211,12 +4211,12 @@
       <c r="AF30" s="52"/>
       <c r="AG30" s="52"/>
     </row>
-    <row r="31" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG31" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="77" t="s">
         <v>375</v>
       </c>
@@ -4227,7 +4227,7 @@
       <c r="E32" s="50"/>
       <c r="G32" s="36"/>
     </row>
-    <row r="33" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="77" t="s">
         <v>376</v>
       </c>
@@ -4238,7 +4238,7 @@
       <c r="E33" s="50"/>
       <c r="G33" s="36"/>
     </row>
-    <row r="34" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="77" t="s">
         <v>377</v>
       </c>
@@ -4249,7 +4249,7 @@
       <c r="E34" s="50"/>
       <c r="G34" s="36"/>
     </row>
-    <row r="35" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="77" t="s">
         <v>393</v>
       </c>
@@ -4260,7 +4260,7 @@
       <c r="E35" s="50"/>
       <c r="G35" s="36"/>
     </row>
-    <row r="36" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="77" t="s">
         <v>394</v>
       </c>
@@ -4271,12 +4271,12 @@
       <c r="E36" s="50"/>
       <c r="G36" s="36"/>
     </row>
-    <row r="37" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG37" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="51"/>
       <c r="C38" s="51"/>
       <c r="D38" s="51"/>
@@ -4310,12 +4310,12 @@
       <c r="AF38" s="52"/>
       <c r="AG38" s="52"/>
     </row>
-    <row r="39" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG39" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="81" t="s">
         <v>427</v>
       </c>
@@ -4326,7 +4326,7 @@
       <c r="E40" s="37"/>
       <c r="G40" s="36"/>
     </row>
-    <row r="41" spans="2:33" s="20" customFormat="1" ht="30.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:33" s="20" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="38" t="s">
         <v>378</v>
       </c>
@@ -4336,7 +4336,7 @@
       </c>
       <c r="G41" s="36"/>
     </row>
-    <row r="42" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="77" t="s">
         <v>333</v>
       </c>
@@ -4346,7 +4346,7 @@
       </c>
       <c r="G42" s="36"/>
     </row>
-    <row r="43" spans="2:33" s="20" customFormat="1" ht="45.7" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:33" s="20" customFormat="1" ht="46.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B43" s="38" t="s">
         <v>303</v>
       </c>
@@ -4356,12 +4356,12 @@
       </c>
       <c r="G43" s="36"/>
     </row>
-    <row r="44" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG44" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="51"/>
       <c r="C45" s="51"/>
       <c r="D45" s="51"/>
@@ -4395,13 +4395,13 @@
       <c r="AF45" s="52"/>
       <c r="AG45" s="52"/>
     </row>
-    <row r="46" spans="2:33" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="49"/>
       <c r="AG46" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:33" s="30" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:33" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="38" t="s">
         <v>379</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:33" s="20" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:33" s="20" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B48" s="58" t="s">
         <v>343</v>
       </c>
@@ -4424,7 +4424,7 @@
       <c r="E48" s="30"/>
       <c r="G48" s="36"/>
     </row>
-    <row r="49" spans="2:33" s="20" customFormat="1" ht="30.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:33" s="20" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="38" t="s">
         <v>344</v>
       </c>
@@ -4435,7 +4435,7 @@
       <c r="E49" s="30"/>
       <c r="G49" s="36"/>
     </row>
-    <row r="50" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="38" t="s">
         <v>359</v>
       </c>
@@ -4445,7 +4445,7 @@
       </c>
       <c r="G50" s="36"/>
     </row>
-    <row r="51" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="38" t="s">
         <v>361</v>
       </c>
@@ -4455,7 +4455,7 @@
       </c>
       <c r="G51" s="36"/>
     </row>
-    <row r="52" spans="2:33" s="20" customFormat="1" ht="31" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="2:33" s="20" customFormat="1" ht="47.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="38" t="s">
         <v>380</v>
       </c>
@@ -4465,7 +4465,7 @@
       </c>
       <c r="G52" s="36"/>
     </row>
-    <row r="53" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="81" t="s">
         <v>426</v>
       </c>
@@ -4475,7 +4475,7 @@
       </c>
       <c r="G53" s="36"/>
     </row>
-    <row r="54" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="77" t="s">
         <v>318</v>
       </c>
@@ -4484,7 +4484,7 @@
       </c>
       <c r="G54" s="36"/>
     </row>
-    <row r="55" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="77" t="s">
         <v>319</v>
       </c>
@@ -4493,7 +4493,7 @@
       </c>
       <c r="G55" s="36"/>
     </row>
-    <row r="56" spans="2:33" s="20" customFormat="1" ht="45.7" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:33" s="20" customFormat="1" ht="46.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B56" s="38" t="s">
         <v>370</v>
       </c>
@@ -4502,12 +4502,12 @@
       </c>
       <c r="G56" s="36"/>
     </row>
-    <row r="57" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="50"/>
       <c r="C57" s="50"/>
       <c r="D57" s="50"/>
     </row>
-    <row r="58" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="51"/>
       <c r="C58" s="51"/>
       <c r="D58" s="51"/>
@@ -4541,12 +4541,12 @@
       <c r="AF58" s="52"/>
       <c r="AG58" s="52"/>
     </row>
-    <row r="59" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AG59" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="77" t="s">
         <v>381</v>
       </c>
@@ -4555,7 +4555,7 @@
       </c>
       <c r="G60" s="36"/>
     </row>
-    <row r="61" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="77" t="s">
         <v>382</v>
       </c>
@@ -4564,7 +4564,7 @@
       </c>
       <c r="G61" s="36"/>
     </row>
-    <row r="62" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="38" t="s">
         <v>383</v>
       </c>
@@ -4573,7 +4573,7 @@
       </c>
       <c r="G62" s="36"/>
     </row>
-    <row r="63" spans="2:33" s="20" customFormat="1" ht="15.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:33" s="20" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="38" t="s">
         <v>384</v>
       </c>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="G63" s="36"/>
     </row>
-    <row r="64" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="77" t="s">
         <v>315</v>
       </c>
@@ -4591,7 +4591,7 @@
       </c>
       <c r="G64" s="36"/>
     </row>
-    <row r="65" spans="2:7" s="20" customFormat="1" ht="31" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="2:7" s="20" customFormat="1" ht="32.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="77" t="s">
         <v>397</v>
       </c>
@@ -4600,7 +4600,7 @@
       </c>
       <c r="G65" s="36"/>
     </row>
-    <row r="66" spans="2:7" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="2:7" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="77" t="s">
         <v>316</v>
       </c>
@@ -4609,7 +4609,7 @@
       </c>
       <c r="G66" s="36"/>
     </row>
-    <row r="67" spans="2:7" s="20" customFormat="1" ht="15.7" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="2:7" s="20" customFormat="1" ht="31.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B67" s="77" t="s">
         <v>398</v>
       </c>
@@ -4618,15 +4618,15 @@
       </c>
       <c r="G67" s="36"/>
     </row>
-    <row r="68" spans="2:7" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="50"/>
       <c r="D68" s="39"/>
     </row>
-    <row r="69" spans="2:7" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:7" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G69" s="36"/>
     </row>
-    <row r="70" spans="2:7" s="40" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="71" spans="2:7" s="20" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:7" s="40" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="2:7" s="20" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B71" s="77" t="s">
         <v>385</v>
       </c>
@@ -4635,7 +4635,7 @@
       </c>
       <c r="G71" s="36"/>
     </row>
-    <row r="72" spans="2:7" s="20" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
+    <row r="72" spans="2:7" s="20" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B72" s="77" t="s">
         <v>386</v>
       </c>
@@ -4644,7 +4644,7 @@
       </c>
       <c r="G72" s="36"/>
     </row>
-    <row r="73" spans="2:7" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="73" spans="2:7" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="38" t="s">
         <v>425</v>
       </c>
@@ -4819,18 +4819,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="45.703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.41015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5859375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="45.703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="45.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:18" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="21" t="s">
         <v>14</v>
       </c>
@@ -4838,7 +4838,7 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G3" s="4"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -4852,7 +4852,7 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -4860,15 +4860,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" s="16"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -4876,7 +4876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>20</v>
       </c>
@@ -4887,7 +4887,7 @@
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>22</v>
       </c>
@@ -4898,7 +4898,7 @@
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>24</v>
       </c>
@@ -4909,7 +4909,7 @@
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
         <v>26</v>
       </c>
@@ -4920,15 +4920,15 @@
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="20"/>
       <c r="C14" s="23"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" s="20"/>
       <c r="C15" s="23"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
         <v>28</v>
       </c>
@@ -4945,7 +4945,7 @@
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="G17" s="4"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -4959,7 +4959,7 @@
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -4990,7 +4990,7 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
     </row>
-    <row r="19" spans="2:18" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:18" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B19" s="20">
         <v>1</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="20">
         <v>2</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:18" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:18" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="20">
         <v>3</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="20">
         <v>4</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="2:18" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:18" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" s="20">
         <v>5</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="20">
         <v>6</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="20">
         <v>7</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="2:18" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:18" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B26" s="20">
         <v>8</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="20">
         <v>9</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="20">
         <v>10</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:18" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B29" s="20">
         <v>11</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="20">
         <v>12</v>
       </c>
@@ -5240,7 +5240,7 @@
       </c>
       <c r="G30" s="23"/>
     </row>
-    <row r="31" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="20">
         <v>13</v>
       </c>
@@ -5259,7 +5259,7 @@
       </c>
       <c r="G31" s="23"/>
     </row>
-    <row r="32" spans="2:18" s="20" customFormat="1" ht="157.69999999999999" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:18" s="20" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="B32" s="20">
         <v>14</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B33" s="20">
         <v>15</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="2:7" s="20" customFormat="1" ht="86" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B34" s="20">
         <v>16</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B35" s="20">
         <v>17</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="20">
         <v>18</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="2:7" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="20">
         <v>19</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B38" s="20">
         <v>20</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B39" s="20">
         <v>21</v>
       </c>
@@ -5425,7 +5425,7 @@
       </c>
       <c r="G39" s="23"/>
     </row>
-    <row r="40" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B40" s="20">
         <v>22</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B41" s="20">
         <v>23</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="20">
         <v>24</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="2:7" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B43" s="20">
         <v>25</v>
       </c>
@@ -5509,7 +5509,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="2:7" s="20" customFormat="1" ht="114.7" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:7" s="20" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="B44" s="20">
         <v>26</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B45" s="20">
         <v>27</v>
       </c>
@@ -5549,7 +5549,7 @@
       </c>
       <c r="G45" s="23"/>
     </row>
-    <row r="46" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="20">
         <v>28</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="2:7" s="20" customFormat="1" ht="114.7" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:7" s="20" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="B47" s="20">
         <v>29</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B48" s="20">
         <v>30</v>
       </c>
@@ -5610,7 +5610,7 @@
       </c>
       <c r="G48" s="23"/>
     </row>
-    <row r="49" spans="2:12" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:12" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B49" s="20">
         <v>31</v>
       </c>
@@ -5629,7 +5629,7 @@
       </c>
       <c r="G49" s="23"/>
     </row>
-    <row r="50" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:12" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B50" s="20">
         <v>32</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:12" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B51" s="20">
         <v>33</v>
       </c>
@@ -5669,7 +5669,7 @@
       </c>
       <c r="G51" s="23"/>
     </row>
-    <row r="52" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B52" s="20">
         <v>34</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B53" s="20">
         <v>35</v>
       </c>
@@ -5709,7 +5709,7 @@
       </c>
       <c r="G53" s="23"/>
     </row>
-    <row r="54" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="20">
         <v>36</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="20">
         <v>37</v>
       </c>
@@ -5749,7 +5749,7 @@
       </c>
       <c r="G55" s="23"/>
     </row>
-    <row r="56" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="20">
         <v>38</v>
       </c>
@@ -5765,7 +5765,7 @@
       </c>
       <c r="G56" s="23"/>
     </row>
-    <row r="57" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:12" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="B57" s="20">
         <v>39</v>
       </c>
@@ -5785,7 +5785,7 @@
       <c r="G57" s="23"/>
       <c r="L57" s="27"/>
     </row>
-    <row r="58" spans="2:12" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:12" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="20">
         <v>40</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="2:12" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B59" s="20">
         <v>41</v>
       </c>
@@ -5827,7 +5827,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B60" s="20">
         <v>42</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="2:12" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:12" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" s="20">
         <v>43</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="20">
         <v>44</v>
       </c>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="G62" s="23"/>
     </row>
-    <row r="63" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B63" s="20">
         <v>45</v>
       </c>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="G63" s="23"/>
     </row>
-    <row r="64" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:12" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B64" s="20">
         <v>46</v>
       </c>
@@ -5926,7 +5926,7 @@
       </c>
       <c r="G64" s="23"/>
     </row>
-    <row r="65" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B65" s="20">
         <v>47</v>
       </c>
@@ -5945,7 +5945,7 @@
       </c>
       <c r="G65" s="23"/>
     </row>
-    <row r="66" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="66" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="20">
         <v>48</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="20">
         <v>49</v>
       </c>
@@ -5985,7 +5985,7 @@
       </c>
       <c r="G67" s="23"/>
     </row>
-    <row r="68" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="20">
         <v>50</v>
       </c>
@@ -6004,7 +6004,7 @@
       </c>
       <c r="G68" s="23"/>
     </row>
-    <row r="69" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="20">
         <v>51</v>
       </c>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="G69" s="23"/>
     </row>
-    <row r="70" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="20">
         <v>52</v>
       </c>
@@ -6042,7 +6042,7 @@
       </c>
       <c r="G70" s="23"/>
     </row>
-    <row r="71" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="71" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B71" s="20">
         <v>53</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="2:7" s="20" customFormat="1" ht="114.7" x14ac:dyDescent="0.5">
+    <row r="72" spans="2:7" s="20" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="B72" s="20">
         <v>54</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="73" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B73" s="20">
         <v>55</v>
       </c>
@@ -6105,7 +6105,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="74" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B74" s="20">
         <v>56</v>
       </c>
@@ -6126,7 +6126,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="75" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="75" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B75" s="20">
         <v>57</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="76" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B76" s="20">
         <v>58</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="77" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="77" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B77" s="20">
         <v>59</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="78" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="78" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B78" s="20">
         <v>60</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="79" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B79" s="20">
         <v>61</v>
       </c>
@@ -6231,7 +6231,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="80" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="80" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B80" s="20">
         <v>62</v>
       </c>
@@ -6250,7 +6250,7 @@
       </c>
       <c r="G80" s="23"/>
     </row>
-    <row r="81" spans="2:7" s="20" customFormat="1" ht="172" x14ac:dyDescent="0.5">
+    <row r="81" spans="2:7" s="20" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="B81" s="20">
         <v>63</v>
       </c>
@@ -6271,7 +6271,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="82" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B82" s="20">
         <v>64</v>
       </c>
@@ -6292,7 +6292,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="83" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="83" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="20">
         <v>65</v>
       </c>
@@ -6311,7 +6311,7 @@
       </c>
       <c r="G83" s="23"/>
     </row>
-    <row r="84" spans="2:7" ht="43" x14ac:dyDescent="0.5">
+    <row r="84" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B84" s="20">
         <v>66</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="85" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B85" s="20">
         <v>67</v>
       </c>
@@ -6351,7 +6351,7 @@
       </c>
       <c r="G85" s="23"/>
     </row>
-    <row r="86" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="86" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B86" s="20">
         <v>68</v>
       </c>
@@ -6372,7 +6372,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="87" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="87" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B87" s="20">
         <v>69</v>
       </c>
@@ -6393,7 +6393,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="88" spans="2:7" s="20" customFormat="1" ht="229.35" x14ac:dyDescent="0.5">
+    <row r="88" spans="2:7" s="20" customFormat="1" ht="285" x14ac:dyDescent="0.25">
       <c r="B88" s="20">
         <v>70</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="89" spans="2:7" s="20" customFormat="1" ht="258" x14ac:dyDescent="0.5">
+    <row r="89" spans="2:7" s="20" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="B89" s="20" t="s">
         <v>336</v>
       </c>
@@ -6435,7 +6435,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="90" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="90" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="20" t="s">
         <v>339</v>
       </c>
@@ -6456,7 +6456,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="91" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="91" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B91" s="20" t="s">
         <v>342</v>
       </c>
@@ -6475,7 +6475,7 @@
       </c>
       <c r="G91" s="59"/>
     </row>
-    <row r="92" spans="2:7" s="20" customFormat="1" ht="186.35" x14ac:dyDescent="0.5">
+    <row r="92" spans="2:7" s="20" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="B92" s="20">
         <v>71</v>
       </c>
@@ -6496,7 +6496,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="93" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="93" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B93" s="20">
         <v>71</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="94" spans="2:7" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="94" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B94" s="20">
         <v>72</v>
       </c>
@@ -6538,7 +6538,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="95" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="95" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B95" s="20">
         <v>73</v>
       </c>
@@ -6557,7 +6557,7 @@
       </c>
       <c r="G95" s="23"/>
     </row>
-    <row r="96" spans="2:7" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="96" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B96" s="20">
         <v>74</v>
       </c>
@@ -6578,7 +6578,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="97" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="97" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B97" s="20">
         <v>75</v>
       </c>
@@ -6597,7 +6597,7 @@
       </c>
       <c r="G97" s="23"/>
     </row>
-    <row r="98" spans="2:7" s="20" customFormat="1" ht="129" x14ac:dyDescent="0.5">
+    <row r="98" spans="2:7" s="20" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="B98" s="20">
         <v>76</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="99" spans="2:7" s="20" customFormat="1" ht="329.7" x14ac:dyDescent="0.5">
+    <row r="99" spans="2:7" s="20" customFormat="1" ht="390" x14ac:dyDescent="0.25">
       <c r="B99" s="20">
         <v>77</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="100" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="100" spans="2:7" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B100" s="20">
         <v>78</v>
       </c>
@@ -6660,7 +6660,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="101" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="101" spans="2:7" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B101" s="20">
         <v>79</v>
       </c>
@@ -6681,7 +6681,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="102" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="102" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B102" s="20">
         <v>80</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="103" spans="2:7" s="20" customFormat="1" ht="86" x14ac:dyDescent="0.5">
+    <row r="103" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B103" s="20">
         <v>81</v>
       </c>
@@ -6723,7 +6723,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="104" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="104" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="20">
         <v>82</v>
       </c>
@@ -6742,7 +6742,7 @@
       </c>
       <c r="G104" s="23"/>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="20">
         <v>83</v>
       </c>
@@ -6761,7 +6761,7 @@
       </c>
       <c r="G105" s="23"/>
     </row>
-    <row r="106" spans="2:7" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="106" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B106" s="20">
         <v>84</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="107" spans="2:7" ht="43" x14ac:dyDescent="0.5">
+    <row r="107" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B107" s="20">
         <v>85</v>
       </c>
@@ -6801,7 +6801,7 @@
       </c>
       <c r="G107" s="23"/>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="20">
         <v>86</v>
       </c>
@@ -6820,7 +6820,7 @@
       </c>
       <c r="G108" s="23"/>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="109" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B109" s="20">
         <v>87</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="110" spans="2:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="110" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B110" s="20">
         <v>88</v>
       </c>
@@ -6860,7 +6860,7 @@
       </c>
       <c r="G110" s="23"/>
     </row>
-    <row r="111" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="111" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B111" s="20">
         <v>89</v>
       </c>
@@ -6881,7 +6881,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="112" spans="2:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="112" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B112" s="20">
         <v>90</v>
       </c>
@@ -6900,7 +6900,7 @@
       </c>
       <c r="G112" s="23"/>
     </row>
-    <row r="113" spans="2:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="113" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B113" s="20">
         <v>91</v>
       </c>
@@ -6919,7 +6919,7 @@
       </c>
       <c r="G113" s="23"/>
     </row>
-    <row r="114" spans="2:7" ht="43" x14ac:dyDescent="0.5">
+    <row r="114" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B114" s="20">
         <v>92</v>
       </c>
@@ -6938,7 +6938,7 @@
       </c>
       <c r="G114" s="23"/>
     </row>
-    <row r="115" spans="2:7" ht="129" x14ac:dyDescent="0.5">
+    <row r="115" spans="2:7" ht="135" x14ac:dyDescent="0.25">
       <c r="B115" s="20">
         <v>93</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" s="20">
         <v>94</v>
       </c>
@@ -6969,7 +6969,7 @@
       <c r="F116" s="23"/>
       <c r="G116" s="23"/>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B117" s="20">
         <v>95</v>
       </c>
@@ -6979,7 +6979,7 @@
       <c r="F117" s="23"/>
       <c r="G117" s="23"/>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B118" s="20">
         <v>96</v>
       </c>
@@ -6989,7 +6989,7 @@
       <c r="F118" s="23"/>
       <c r="G118" s="23"/>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B119" s="20">
         <v>97</v>
       </c>
@@ -6999,7 +6999,7 @@
       <c r="F119" s="23"/>
       <c r="G119" s="23"/>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B120" s="20">
         <v>98</v>
       </c>
@@ -7009,7 +7009,7 @@
       <c r="F120" s="23"/>
       <c r="G120" s="23"/>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B121" s="20">
         <v>99</v>
       </c>
@@ -7019,7 +7019,7 @@
       <c r="F121" s="23"/>
       <c r="G121" s="23"/>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B122" s="20">
         <v>100</v>
       </c>
@@ -7053,21 +7053,21 @@
       <selection activeCell="B218" sqref="B218"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
-    <col min="2" max="2" width="92.29296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.1171875" customWidth="1"/>
-    <col min="4" max="5" width="16.703125" customWidth="1"/>
-    <col min="6" max="17" width="16.703125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="92.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" customWidth="1"/>
+    <col min="4" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="17" width="16.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:17" s="71" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="71" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -7087,7 +7087,7 @@
       <c r="P4"/>
       <c r="Q4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -7106,7 +7106,7 @@
       <c r="P5"/>
       <c r="Q5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -7125,7 +7125,7 @@
       <c r="P6"/>
       <c r="Q6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -7138,12 +7138,12 @@
       <c r="P7"/>
       <c r="Q7"/>
     </row>
-    <row r="8" spans="1:17" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:17" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="72" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G9"/>
       <c r="H9"/>
       <c r="I9"/>
@@ -7156,7 +7156,7 @@
       <c r="P9"/>
       <c r="Q9"/>
     </row>
-    <row r="10" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
         <v>187</v>
       </c>
@@ -7178,7 +7178,7 @@
       <c r="P10" s="73"/>
       <c r="Q10" s="73"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>190</v>
       </c>
@@ -7192,7 +7192,7 @@
       </c>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>192</v>
       </c>
@@ -7206,7 +7206,7 @@
       </c>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>191</v>
       </c>
@@ -7220,80 +7220,80 @@
       </c>
       <c r="G13"/>
     </row>
-    <row r="15" spans="1:17" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:17" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B15" s="72" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="16" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="16"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="16" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="16" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f t="shared" ref="B37:B43" si="0">D38</f>
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
@@ -7312,7 +7312,7 @@
       <c r="P37"/>
       <c r="Q37"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>Gas Control Device/Control System Component</v>
@@ -7331,7 +7331,7 @@
       <c r="P38"/>
       <c r="Q38"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f t="shared" si="0"/>
         <v>Landfill Surface: Daily Cover</v>
@@ -7349,7 +7349,7 @@
       <c r="P39"/>
       <c r="Q39"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>Landfill Surface: Final Cover</v>
@@ -7367,7 +7367,7 @@
       <c r="P40"/>
       <c r="Q40"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>Landfill Surface: Intermediate Cover</v>
@@ -7385,7 +7385,7 @@
       <c r="P41"/>
       <c r="Q41"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>Leachate Management System</v>
@@ -7403,7 +7403,7 @@
       <c r="P42"/>
       <c r="Q42"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
@@ -7421,25 +7421,25 @@
       <c r="P43"/>
       <c r="Q43"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D44" s="7" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45" s="16" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" s="16"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="48" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="67" t="str" cm="1">
         <f t="array" ref="B48:B58">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn.TOCOL(C64:M70, 1)))</f>
         <v>Collection system downtime</v>
@@ -7447,89 +7447,89 @@
       <c r="E48" s="7"/>
       <c r="Q48"/>
     </row>
-    <row r="49" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="69" t="str">
         <v>Construction - New Well Installation</v>
       </c>
       <c r="E49" s="7"/>
       <c r="Q49"/>
     </row>
-    <row r="50" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="70" t="str">
         <v>Construction - Well Raising or Horizontal Extension</v>
       </c>
       <c r="E50" s="7"/>
       <c r="Q50"/>
     </row>
-    <row r="51" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="68" t="str">
         <v>Cover integrity</v>
       </c>
       <c r="E51" s="7"/>
       <c r="Q51"/>
     </row>
-    <row r="52" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="67" t="str">
         <v>Cover-related Construction (Excavation/ Exposed Operations/ Re-grading)</v>
       </c>
       <c r="E52" s="7"/>
       <c r="Q52"/>
     </row>
-    <row r="53" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="68" t="str">
         <v>Cracked/Broken Seal</v>
       </c>
       <c r="E53" s="7"/>
       <c r="Q53"/>
     </row>
-    <row r="54" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="67" t="str">
         <v>Damaged component</v>
       </c>
       <c r="E54" s="7"/>
       <c r="Q54"/>
     </row>
-    <row r="55" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="67" t="str">
         <v>Insufficient vacuum</v>
       </c>
       <c r="E55" s="7"/>
       <c r="Q55"/>
     </row>
-    <row r="56" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="69" t="str">
         <v>Offline Gas Collection Well(s)</v>
       </c>
       <c r="E56" s="7"/>
       <c r="Q56"/>
     </row>
-    <row r="57" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="70" t="str">
         <v>Other</v>
       </c>
       <c r="E57" s="7"/>
       <c r="Q57"/>
     </row>
-    <row r="58" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="68" t="str">
         <v>Uncontrolled Area (no gas collection infrastructure)</v>
       </c>
       <c r="E58" s="7"/>
       <c r="Q58"/>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B60" s="16" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="12" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="2:17" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="62" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B62" s="3" t="s">
         <v>176</v>
       </c>
@@ -7537,7 +7537,7 @@
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="2:17" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>177</v>
       </c>
@@ -7547,7 +7547,7 @@
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="2:17" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:17" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="6" t="s">
         <v>399</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="10" t="s">
         <v>167</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="66" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
         <v>168</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="67" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="6" t="s">
         <v>169</v>
       </c>
@@ -7687,7 +7687,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="68" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="10" t="s">
         <v>170</v>
       </c>
@@ -7711,7 +7711,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="69" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
         <v>186</v>
       </c>
@@ -7741,7 +7741,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="70" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="6" t="s">
         <v>13</v>
       </c>
@@ -7763,12 +7763,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B72" s="16" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B74" t="str" cm="1">
         <f t="array" ref="B74:C125">_xlfn.HSTACK(_xlfn.TOCOL(_xlfn.IFS(C64:M70&lt;&gt;"",B64:B70),3),_xlfn.TOCOL(C64:M70,1))</f>
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
@@ -7778,7 +7778,7 @@
       </c>
       <c r="G74"/>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B75" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7787,7 +7787,7 @@
       </c>
       <c r="G75"/>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B76" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7796,7 +7796,7 @@
       </c>
       <c r="G76"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B77" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7805,7 +7805,7 @@
       </c>
       <c r="G77"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B78" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7814,7 +7814,7 @@
       </c>
       <c r="G78"/>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B79" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7823,7 +7823,7 @@
       </c>
       <c r="G79"/>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B80" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7832,7 +7832,7 @@
       </c>
       <c r="G80"/>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7841,7 +7841,7 @@
       </c>
       <c r="G81"/>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7850,7 +7850,7 @@
       </c>
       <c r="G82"/>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7859,7 +7859,7 @@
       </c>
       <c r="G83"/>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7868,7 +7868,7 @@
       </c>
       <c r="G84"/>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7877,7 +7877,7 @@
       </c>
       <c r="G85"/>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7886,7 +7886,7 @@
       </c>
       <c r="G86"/>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7895,7 +7895,7 @@
       </c>
       <c r="G87"/>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7904,7 +7904,7 @@
       </c>
       <c r="G88"/>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7913,7 +7913,7 @@
       </c>
       <c r="G89"/>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7922,7 +7922,7 @@
       </c>
       <c r="G90"/>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7931,7 +7931,7 @@
       </c>
       <c r="G91"/>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7940,7 +7940,7 @@
       </c>
       <c r="G92"/>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7949,7 +7949,7 @@
       </c>
       <c r="G93"/>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7958,7 +7958,7 @@
       </c>
       <c r="G94"/>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7967,7 +7967,7 @@
       </c>
       <c r="G95"/>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7976,7 +7976,7 @@
       </c>
       <c r="G96"/>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7985,7 +7985,7 @@
       </c>
       <c r="G97"/>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7994,7 +7994,7 @@
       </c>
       <c r="G98"/>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8003,7 +8003,7 @@
       </c>
       <c r="G99"/>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B100" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8012,7 +8012,7 @@
       </c>
       <c r="G100"/>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B101" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8021,7 +8021,7 @@
       </c>
       <c r="G101"/>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8030,7 +8030,7 @@
       </c>
       <c r="G102"/>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8039,7 +8039,7 @@
       </c>
       <c r="G103"/>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8048,7 +8048,7 @@
       </c>
       <c r="G104"/>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8057,7 +8057,7 @@
       </c>
       <c r="G105"/>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8066,7 +8066,7 @@
       </c>
       <c r="G106"/>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8075,7 +8075,7 @@
       </c>
       <c r="G107"/>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8084,7 +8084,7 @@
       </c>
       <c r="G108"/>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8093,7 +8093,7 @@
       </c>
       <c r="G109"/>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B110" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8102,7 +8102,7 @@
       </c>
       <c r="G110"/>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8111,7 +8111,7 @@
       </c>
       <c r="G111"/>
     </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8120,7 +8120,7 @@
       </c>
       <c r="G112"/>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B113" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8129,7 +8129,7 @@
       </c>
       <c r="G113"/>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B114" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8138,7 +8138,7 @@
       </c>
       <c r="G114"/>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B115" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8147,7 +8147,7 @@
       </c>
       <c r="G115"/>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8156,7 +8156,7 @@
       </c>
       <c r="G116"/>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B117" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8165,7 +8165,7 @@
       </c>
       <c r="G117"/>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B118" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8174,7 +8174,7 @@
       </c>
       <c r="G118"/>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B119" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8183,7 +8183,7 @@
       </c>
       <c r="G119"/>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B120" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8192,7 +8192,7 @@
       </c>
       <c r="G120"/>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B121" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8201,7 +8201,7 @@
       </c>
       <c r="G121"/>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B122" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8210,7 +8210,7 @@
       </c>
       <c r="G122"/>
     </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B123" t="str">
         <v>Gas Control Device/Control System Component</v>
       </c>
@@ -8218,7 +8218,7 @@
         <v>Cover-related Construction (Excavation/ Exposed Operations/ Re-grading)</v>
       </c>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B124" t="str">
         <v>Gas Control Device/Control System Component</v>
       </c>
@@ -8227,7 +8227,7 @@
       </c>
       <c r="G124"/>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B125" t="str">
         <v>Gas Control Device/Control System Component</v>
       </c>
@@ -8236,21 +8236,21 @@
       </c>
       <c r="G125"/>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G126"/>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G134"/>
     </row>
-    <row r="135" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="135" spans="2:7" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B135" s="72" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G136"/>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B137" s="17" t="s">
         <v>193</v>
       </c>
@@ -8259,12 +8259,12 @@
       </c>
       <c r="G137"/>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B138" s="16"/>
       <c r="C138" s="16"/>
       <c r="G138"/>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>163</v>
       </c>
@@ -8274,7 +8274,7 @@
       </c>
       <c r="G139"/>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B140" t="str" cm="1">
         <f t="array" ref="B140:B142">_carb_only_table_02[]</f>
         <v>Operator was aware of the leak prior to receiving the CARB plume notification</v>
@@ -8284,7 +8284,7 @@
       </c>
       <c r="G140"/>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B141" t="str">
         <v>Operator detected a leak during follow-up monitoring after receipt of the CARB plume notification</v>
       </c>
@@ -8293,7 +8293,7 @@
       </c>
       <c r="G141"/>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" t="str">
         <v>No leak was detected</v>
       </c>
@@ -8302,18 +8302,18 @@
       </c>
       <c r="G142"/>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G143"/>
     </row>
-    <row r="144" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="144" spans="2:7" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B144" s="72" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G145"/>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B146" s="17" t="s">
         <v>193</v>
       </c>
@@ -8322,12 +8322,12 @@
       </c>
       <c r="G146"/>
     </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147" s="16"/>
       <c r="C147" s="16"/>
       <c r="G147"/>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>163</v>
       </c>
@@ -8337,7 +8337,7 @@
       </c>
       <c r="G148"/>
     </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B149" t="str">
         <f ca="1">IF(C11=B26, "Not applicable as no leak was detected", "")</f>
         <v/>
@@ -8348,7 +8348,7 @@
       </c>
       <c r="G149"/>
     </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B150" t="str" cm="1">
         <f t="array" ref="B150:B153">_carb_only_table_03[]</f>
         <v>Operator was aware of the leak prior to receiving the notification, and/or repairs were in progress on the date of the plume observation</v>
@@ -8359,7 +8359,7 @@
       </c>
       <c r="G150"/>
     </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B151" t="str">
         <v>An unintentional leak  (i.e., the operator was not aware of, and could be repaired if discovered)</v>
       </c>
@@ -8369,7 +8369,7 @@
       </c>
       <c r="G151"/>
     </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B152" t="str">
         <v>An intentional or allowable vent (i.e., the operator was aware of, and/or would not repair)</v>
       </c>
@@ -8379,24 +8379,24 @@
       </c>
       <c r="G152"/>
     </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B153" t="str">
         <v>Due to a temporary activity (i.e., would be resolved without corrective action when the activity is complete)</v>
       </c>
       <c r="G153"/>
     </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G154"/>
     </row>
-    <row r="155" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="155" spans="2:7" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B155" s="72" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G156"/>
     </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B157" s="17" t="s">
         <v>193</v>
       </c>
@@ -8405,12 +8405,12 @@
       </c>
       <c r="G157"/>
     </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B158" s="16"/>
       <c r="C158" s="16"/>
       <c r="G158"/>
     </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>163</v>
       </c>
@@ -8420,7 +8420,7 @@
       </c>
       <c r="G159"/>
     </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B160" t="str">
         <f ca="1">IF(C11=B26, "Not applicable as no leak was detected", "")</f>
         <v/>
@@ -8431,7 +8431,7 @@
       </c>
       <c r="G160"/>
     </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B161" t="str" cm="1">
         <f t="array" ref="B161:B167">_carb_only_table_04[]</f>
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
@@ -8442,7 +8442,7 @@
       </c>
       <c r="G161"/>
     </row>
-    <row r="162" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B162" t="str">
         <v>Gas Control Device/Control System Component</v>
       </c>
@@ -8452,7 +8452,7 @@
       </c>
       <c r="G162"/>
     </row>
-    <row r="163" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B163" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -8462,7 +8462,7 @@
       </c>
       <c r="G163"/>
     </row>
-    <row r="164" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B164" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8472,7 +8472,7 @@
       </c>
       <c r="G164"/>
     </row>
-    <row r="165" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="165" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B165" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8482,7 +8482,7 @@
       </c>
       <c r="G165"/>
     </row>
-    <row r="166" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="166" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B166" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8492,24 +8492,24 @@
       </c>
       <c r="G166"/>
     </row>
-    <row r="167" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="167" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B167" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
       <c r="G167"/>
     </row>
-    <row r="168" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="168" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G168"/>
     </row>
-    <row r="169" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="169" spans="2:7" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B169" s="72" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="170" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="170" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G170"/>
     </row>
-    <row r="171" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B171" s="17" t="s">
         <v>193</v>
       </c>
@@ -8518,12 +8518,12 @@
       </c>
       <c r="G171"/>
     </row>
-    <row r="172" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="172" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B172" s="16"/>
       <c r="C172" s="16"/>
       <c r="G172"/>
     </row>
-    <row r="173" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>163</v>
       </c>
@@ -8533,74 +8533,74 @@
       </c>
       <c r="G173"/>
     </row>
-    <row r="174" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B174" t="str">
         <f ca="1">IF(C11=B26, "Not applicable as no leak was detected", "")</f>
         <v/>
       </c>
       <c r="G174"/>
     </row>
-    <row r="175" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="175" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B175" t="str" cm="1">
         <f t="array" aca="1" ref="B175" ca="1">_xlfn._xlws.FILTER($C$74:$C$125, $B$74:$B$125=C13, "")</f>
         <v/>
       </c>
       <c r="G175"/>
     </row>
-    <row r="176" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G176"/>
     </row>
-    <row r="177" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="177" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G177"/>
     </row>
-    <row r="178" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="178" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G178"/>
     </row>
-    <row r="179" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G179"/>
     </row>
-    <row r="180" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G180"/>
     </row>
-    <row r="181" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G181"/>
     </row>
-    <row r="182" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G182"/>
     </row>
-    <row r="183" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G183"/>
     </row>
-    <row r="184" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G184"/>
     </row>
-    <row r="185" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G185"/>
     </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G186"/>
     </row>
-    <row r="187" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G187"/>
     </row>
-    <row r="188" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G188"/>
     </row>
-    <row r="189" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="189" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G189"/>
     </row>
-    <row r="190" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="190" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G190"/>
     </row>
-    <row r="191" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="191" spans="2:7" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B191" s="72" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="192" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="192" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G192"/>
     </row>
-    <row r="193" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="193" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B193" s="17" t="s">
         <v>193</v>
       </c>
@@ -8609,12 +8609,12 @@
       </c>
       <c r="G193"/>
     </row>
-    <row r="194" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="194" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B194" s="16"/>
       <c r="C194" s="16"/>
       <c r="G194"/>
     </row>
-    <row r="195" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="195" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>163</v>
       </c>
@@ -8624,7 +8624,7 @@
       </c>
       <c r="G195"/>
     </row>
-    <row r="196" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="196" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B196" t="str">
         <f ca="1">IF(C11=B26, "Not applicable as no leak was detected", "")</f>
         <v/>
@@ -8635,65 +8635,65 @@
       </c>
       <c r="G196"/>
     </row>
-    <row r="197" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="197" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>355</v>
       </c>
       <c r="G197"/>
     </row>
-    <row r="198" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="198" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B198" t="str" cm="1">
         <f t="array" aca="1" ref="B198" ca="1">_xlfn._xlws.FILTER($C$74:$C$125, $B$74:$B$125=C13, "")</f>
         <v/>
       </c>
       <c r="G198"/>
     </row>
-    <row r="199" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="199" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G199"/>
     </row>
-    <row r="200" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="200" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G200"/>
     </row>
-    <row r="201" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="201" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G201"/>
     </row>
-    <row r="202" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="202" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G202"/>
     </row>
-    <row r="203" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="203" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G203"/>
     </row>
-    <row r="204" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="204" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G204"/>
     </row>
-    <row r="205" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="205" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G205"/>
     </row>
-    <row r="206" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="206" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G206"/>
     </row>
-    <row r="207" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="207" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G207"/>
     </row>
-    <row r="208" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="208" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G208"/>
     </row>
-    <row r="209" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="209" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G209"/>
     </row>
-    <row r="210" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="210" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G210"/>
     </row>
-    <row r="213" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="213" spans="2:7" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B213" s="72" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="214" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="214" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B214" s="16"/>
       <c r="G214"/>
     </row>
-    <row r="215" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="215" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B215" s="17" t="s">
         <v>193</v>
       </c>
@@ -8702,12 +8702,12 @@
       </c>
       <c r="G215"/>
     </row>
-    <row r="216" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="216" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B216" s="16"/>
       <c r="C216" s="16"/>
       <c r="G216"/>
     </row>
-    <row r="217" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="217" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
         <v>163</v>
       </c>
@@ -8717,7 +8717,7 @@
       </c>
       <c r="G217"/>
     </row>
-    <row r="218" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="218" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B218" t="str" cm="1">
         <f t="array" ref="B218:B219">_carb_only_table_01[]</f>
         <v>Yes</v>
@@ -8727,7 +8727,7 @@
       </c>
       <c r="G218"/>
     </row>
-    <row r="219" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="219" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B219" t="str">
         <v>No</v>
       </c>
@@ -8755,19 +8755,19 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
-    <col min="2" max="3" width="30.703125" customWidth="1"/>
-    <col min="4" max="9" width="8.703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="9" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="14" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:3" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="14" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -8775,7 +8775,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -8783,7 +8783,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -8791,7 +8791,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -8799,7 +8799,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="15" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:3" s="15" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="15" t="s">
         <v>200</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>202</v>
       </c>
@@ -8829,18 +8829,18 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
-    <col min="2" max="3" width="30.703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="3" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="14" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:3" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="14" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -8848,7 +8848,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -8856,7 +8856,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -8864,7 +8864,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -8872,12 +8872,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="10" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="12" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="13" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:3" s="15" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" s="15" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="15" t="s">
         <v>206</v>
       </c>
@@ -8885,7 +8885,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>208</v>
       </c>
@@ -8893,7 +8893,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>210</v>
       </c>
@@ -8912,28 +8912,28 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:F48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:F48"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.703125" customWidth="1"/>
-    <col min="2" max="2" width="25.1171875" customWidth="1"/>
-    <col min="3" max="3" width="16.41015625" customWidth="1"/>
-    <col min="4" max="4" width="32.41015625" customWidth="1"/>
-    <col min="5" max="5" width="16.41015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="99" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:6" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="21" t="s">
         <v>212</v>
       </c>
       <c r="C2" s="22"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -8943,26 +8943,26 @@
       <c r="C4" s="1"/>
       <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="F5" s="19"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="F6" s="19"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="F7" s="19"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="F8" s="19"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F9" s="19"/>
     </row>
-    <row r="10" spans="1:6" s="15" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:6" s="15" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="15" t="s">
         <v>200</v>
       </c>
@@ -8979,7 +8979,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>350</v>
       </c>
@@ -8996,7 +8996,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>350</v>
       </c>
@@ -9013,7 +9013,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>202</v>
       </c>
@@ -9030,7 +9030,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>202</v>
       </c>
@@ -9047,7 +9047,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>202</v>
       </c>
@@ -9064,7 +9064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>202</v>
       </c>
@@ -9081,7 +9081,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>202</v>
       </c>
@@ -9098,7 +9098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>202</v>
       </c>
@@ -9115,7 +9115,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>202</v>
       </c>
@@ -9132,7 +9132,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>202</v>
       </c>
@@ -9149,7 +9149,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>202</v>
       </c>
@@ -9166,7 +9166,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>202</v>
       </c>
@@ -9183,7 +9183,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>202</v>
       </c>
@@ -9200,7 +9200,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>202</v>
       </c>
@@ -9217,7 +9217,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>202</v>
       </c>
@@ -9234,7 +9234,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>202</v>
       </c>
@@ -9251,7 +9251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>202</v>
       </c>
@@ -9268,7 +9268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>202</v>
       </c>
@@ -9285,7 +9285,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>202</v>
       </c>
@@ -9302,7 +9302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>202</v>
       </c>
@@ -9319,7 +9319,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>202</v>
       </c>
@@ -9336,7 +9336,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>202</v>
       </c>
@@ -9353,7 +9353,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>202</v>
       </c>
@@ -9370,7 +9370,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>202</v>
       </c>
@@ -9387,7 +9387,7 @@
         <v>45152</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>202</v>
       </c>
@@ -9404,7 +9404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>202</v>
       </c>
@@ -9421,7 +9421,7 @@
         <v>45277</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>202</v>
       </c>
@@ -9438,7 +9438,7 @@
         <v>45276</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>202</v>
       </c>
@@ -9455,7 +9455,7 @@
         <v>35.321100000000001</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>202</v>
       </c>
@@ -9472,7 +9472,7 @@
         <v>35.321100000000001</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>202</v>
       </c>
@@ -9489,7 +9489,7 @@
         <v>-119.5808</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>202</v>
       </c>
@@ -9506,7 +9506,7 @@
         <v>-119.5808</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>202</v>
       </c>
@@ -9523,7 +9523,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>202</v>
       </c>
@@ -9540,7 +9540,7 @@
         <v>45275</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>202</v>
       </c>
@@ -9557,7 +9557,7 @@
         <v>45468</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>202</v>
       </c>
@@ -9574,7 +9574,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>202</v>
       </c>
@@ -9591,7 +9591,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>202</v>
       </c>
@@ -9608,7 +9608,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>202</v>
       </c>
@@ -9644,29 +9644,29 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="12.703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.87890625" customWidth="1"/>
-    <col min="5" max="5" width="13.703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5859375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.29296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.29296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.29296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="2" spans="2:13" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="21" t="s">
         <v>418</v>
       </c>
       <c r="C2" s="22"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="6" spans="2:13" ht="86" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:13" ht="90" x14ac:dyDescent="0.25">
       <c r="B6" s="78" t="s">
         <v>406</v>
       </c>
@@ -9704,7 +9704,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="80"/>
       <c r="C7" s="80"/>
       <c r="D7" s="80"/>
@@ -9718,7 +9718,7 @@
       <c r="L7" s="80"/>
       <c r="M7" s="80"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="80"/>
       <c r="C8" s="80"/>
       <c r="D8" s="80"/>
@@ -9732,7 +9732,7 @@
       <c r="L8" s="80"/>
       <c r="M8" s="80"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="80"/>
       <c r="C9" s="80"/>
       <c r="D9" s="80"/>
@@ -9746,7 +9746,7 @@
       <c r="L9" s="80"/>
       <c r="M9" s="80"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="80"/>
       <c r="C10" s="80"/>
       <c r="D10" s="80"/>
@@ -9760,7 +9760,7 @@
       <c r="L10" s="80"/>
       <c r="M10" s="80"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="80"/>
       <c r="C11" s="80"/>
       <c r="D11" s="80"/>
@@ -9774,7 +9774,7 @@
       <c r="L11" s="80"/>
       <c r="M11" s="80"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="80"/>
       <c r="C12" s="80"/>
       <c r="D12" s="80"/>
@@ -9788,7 +9788,7 @@
       <c r="L12" s="80"/>
       <c r="M12" s="80"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="80"/>
       <c r="C13" s="80"/>
       <c r="D13" s="80"/>
@@ -9802,7 +9802,7 @@
       <c r="L13" s="80"/>
       <c r="M13" s="80"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="80"/>
       <c r="C14" s="80"/>
       <c r="D14" s="80"/>
@@ -9816,7 +9816,7 @@
       <c r="L14" s="80"/>
       <c r="M14" s="80"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="80"/>
       <c r="C15" s="80"/>
       <c r="D15" s="80"/>
@@ -9830,7 +9830,7 @@
       <c r="L15" s="80"/>
       <c r="M15" s="80"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="80"/>
       <c r="C16" s="80"/>
       <c r="D16" s="80"/>
@@ -9844,7 +9844,7 @@
       <c r="L16" s="80"/>
       <c r="M16" s="80"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="80"/>
       <c r="C17" s="80"/>
       <c r="D17" s="80"/>
@@ -9858,7 +9858,7 @@
       <c r="L17" s="80"/>
       <c r="M17" s="80"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="80"/>
       <c r="C18" s="80"/>
       <c r="D18" s="80"/>
@@ -9872,7 +9872,7 @@
       <c r="L18" s="80"/>
       <c r="M18" s="80"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="80"/>
       <c r="C19" s="80"/>
       <c r="D19" s="80"/>
@@ -9886,7 +9886,7 @@
       <c r="L19" s="80"/>
       <c r="M19" s="80"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="80"/>
       <c r="C20" s="80"/>
       <c r="D20" s="80"/>
@@ -9900,7 +9900,7 @@
       <c r="L20" s="80"/>
       <c r="M20" s="80"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="80"/>
       <c r="C21" s="80"/>
       <c r="D21" s="80"/>
@@ -9914,7 +9914,7 @@
       <c r="L21" s="80"/>
       <c r="M21" s="80"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="80"/>
       <c r="C22" s="80"/>
       <c r="D22" s="80"/>
@@ -9928,7 +9928,7 @@
       <c r="L22" s="80"/>
       <c r="M22" s="80"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="80"/>
       <c r="C23" s="80"/>
       <c r="D23" s="80"/>
@@ -9942,7 +9942,7 @@
       <c r="L23" s="80"/>
       <c r="M23" s="80"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="80"/>
       <c r="C24" s="80"/>
       <c r="D24" s="80"/>
@@ -9956,7 +9956,7 @@
       <c r="L24" s="80"/>
       <c r="M24" s="80"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="80"/>
       <c r="C25" s="80"/>
       <c r="D25" s="80"/>
@@ -9970,7 +9970,7 @@
       <c r="L25" s="80"/>
       <c r="M25" s="80"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="80"/>
       <c r="C26" s="80"/>
       <c r="D26" s="80"/>
@@ -9990,15 +9990,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E9A34E7C7C736409D4BDE6375CCC276" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cf521a6d855790dbe6a6d894ff439cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32" xmlns:ns3="e20ceb87-0d79-402a-b4b9-75d78589c76d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45aa6d812898c4b0f52b4c3685679ce" ns2:_="" ns3:_="">
     <xsd:import namespace="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
@@ -10233,6 +10224,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -10245,14 +10245,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC83B422-5B73-4269-9006-1DDE9C149499}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10267,6 +10259,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updating how wtform selectors are created
</commit_message>
<xml_diff>
--- a/feedback_forms/current_versions/landfill_operator_feedback_v070.xlsx
+++ b/feedback_forms/current_versions/landfill_operator_feedback_v070.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carb-my.sharepoint.com/personal/tony_held_arb_ca_gov/Documents/code/pycharm/feedback_portal/feedback_forms/current_versions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1058FBB9-DD57-4A6E-B0E3-E8E723D41AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{1058FBB9-DD57-4A6E-B0E3-E8E723D41AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D17F6732-970B-43B9-9905-74A25043ED0A}"/>
   <bookViews>
-    <workbookView xWindow="-25110" yWindow="1635" windowWidth="24195" windowHeight="11655" tabRatio="705" activeTab="5" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
+    <workbookView xWindow="1440" yWindow="867" windowWidth="19200" windowHeight="11093" tabRatio="705" activeTab="5" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="6" r:id="rId1"/>
@@ -3819,17 +3819,17 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="65.7109375" style="19" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="65.7109375" style="19" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="4.1171875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="65.703125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="4.703125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="65.703125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="4.1171875" style="19" customWidth="1"/>
     <col min="6" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
@@ -3865,7 +3865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:33" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:33" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.5">
       <c r="B2" s="31" t="s">
         <v>1</v>
       </c>
@@ -3874,7 +3874,7 @@
       <c r="E2" s="31"/>
       <c r="F2" s="49"/>
     </row>
-    <row r="3" spans="2:33" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:33" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.5">
       <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
@@ -3883,13 +3883,13 @@
       <c r="E3" s="31"/>
       <c r="F3" s="50"/>
     </row>
-    <row r="4" spans="2:33" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:33" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="32"/>
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
       <c r="E4" s="33"/>
     </row>
-    <row r="5" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
       <c r="D6" s="51"/>
@@ -3959,12 +3959,12 @@
       <c r="AF6" s="52"/>
       <c r="AG6" s="52"/>
     </row>
-    <row r="7" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="AG7" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B8" s="75" t="s">
         <v>389</v>
       </c>
@@ -3973,7 +3973,7 @@
       <c r="E8" s="35"/>
       <c r="F8" s="49"/>
     </row>
-    <row r="9" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B9" s="62" t="s">
         <v>284</v>
       </c>
@@ -3982,7 +3982,7 @@
       <c r="E9" s="35"/>
       <c r="F9" s="49"/>
     </row>
-    <row r="10" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B10" s="63" t="s">
         <v>285</v>
       </c>
@@ -3991,7 +3991,7 @@
       <c r="E10" s="35"/>
       <c r="F10" s="49"/>
     </row>
-    <row r="11" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:33" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B11" s="64" t="s">
         <v>286</v>
       </c>
@@ -4000,7 +4000,7 @@
       <c r="E11" s="35"/>
       <c r="F11" s="49"/>
     </row>
-    <row r="12" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B12" s="61" t="s">
         <v>282</v>
       </c>
@@ -4009,7 +4009,7 @@
       <c r="E12" s="35"/>
       <c r="F12" s="49"/>
     </row>
-    <row r="13" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B13" s="61" t="s">
         <v>283</v>
       </c>
@@ -4018,7 +4018,7 @@
       <c r="E13" s="35"/>
       <c r="F13" s="49"/>
     </row>
-    <row r="14" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B14" s="75" t="s">
         <v>390</v>
       </c>
@@ -4027,7 +4027,7 @@
       <c r="E14" s="35"/>
       <c r="F14" s="49"/>
     </row>
-    <row r="15" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B15" s="75" t="s">
         <v>391</v>
       </c>
@@ -4036,7 +4036,7 @@
       <c r="E15" s="35"/>
       <c r="F15" s="49"/>
     </row>
-    <row r="16" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B16" s="61" t="s">
         <v>287</v>
       </c>
@@ -4045,7 +4045,7 @@
       <c r="E16" s="35"/>
       <c r="F16" s="49"/>
     </row>
-    <row r="17" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B17" s="75" t="s">
         <v>392</v>
       </c>
@@ -4054,7 +4054,7 @@
       <c r="E17" s="35"/>
       <c r="F17" s="49"/>
     </row>
-    <row r="18" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B18" s="65" t="s">
         <v>288</v>
       </c>
@@ -4063,12 +4063,12 @@
       <c r="E18" s="35"/>
       <c r="F18" s="49"/>
     </row>
-    <row r="20" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="AG20" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="51"/>
@@ -4102,12 +4102,12 @@
       <c r="AF21" s="52"/>
       <c r="AG21" s="52"/>
     </row>
-    <row r="22" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="AG22" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B23" s="74" t="s">
         <v>371</v>
       </c>
@@ -4118,7 +4118,7 @@
       <c r="E23" s="48"/>
       <c r="G23" s="36"/>
     </row>
-    <row r="24" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B24" s="74" t="s">
         <v>372</v>
       </c>
@@ -4128,7 +4128,7 @@
       </c>
       <c r="E24" s="35"/>
     </row>
-    <row r="25" spans="2:33" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:33" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B25" s="74" t="s">
         <v>373</v>
       </c>
@@ -4138,7 +4138,7 @@
       </c>
       <c r="E25" s="35"/>
     </row>
-    <row r="26" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B26" s="75" t="s">
         <v>395</v>
       </c>
@@ -4149,7 +4149,7 @@
       <c r="E26" s="48"/>
       <c r="G26" s="36"/>
     </row>
-    <row r="27" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B27" s="74" t="s">
         <v>374</v>
       </c>
@@ -4160,7 +4160,7 @@
       <c r="E27" s="48"/>
       <c r="G27" s="36"/>
     </row>
-    <row r="28" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B28" s="76" t="s">
         <v>396</v>
       </c>
@@ -4172,12 +4172,12 @@
       <c r="F28" s="49"/>
       <c r="G28" s="36"/>
     </row>
-    <row r="29" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="AG29" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
       <c r="D30" s="51"/>
@@ -4211,12 +4211,12 @@
       <c r="AF30" s="52"/>
       <c r="AG30" s="52"/>
     </row>
-    <row r="31" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="AG31" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B32" s="77" t="s">
         <v>375</v>
       </c>
@@ -4227,7 +4227,7 @@
       <c r="E32" s="50"/>
       <c r="G32" s="36"/>
     </row>
-    <row r="33" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B33" s="77" t="s">
         <v>376</v>
       </c>
@@ -4238,7 +4238,7 @@
       <c r="E33" s="50"/>
       <c r="G33" s="36"/>
     </row>
-    <row r="34" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B34" s="77" t="s">
         <v>377</v>
       </c>
@@ -4249,7 +4249,7 @@
       <c r="E34" s="50"/>
       <c r="G34" s="36"/>
     </row>
-    <row r="35" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B35" s="77" t="s">
         <v>393</v>
       </c>
@@ -4260,7 +4260,7 @@
       <c r="E35" s="50"/>
       <c r="G35" s="36"/>
     </row>
-    <row r="36" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B36" s="77" t="s">
         <v>394</v>
       </c>
@@ -4271,12 +4271,12 @@
       <c r="E36" s="50"/>
       <c r="G36" s="36"/>
     </row>
-    <row r="37" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="AG37" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B38" s="51"/>
       <c r="C38" s="51"/>
       <c r="D38" s="51"/>
@@ -4310,12 +4310,12 @@
       <c r="AF38" s="52"/>
       <c r="AG38" s="52"/>
     </row>
-    <row r="39" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="AG39" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B40" s="81" t="s">
         <v>427</v>
       </c>
@@ -4326,7 +4326,7 @@
       <c r="E40" s="37"/>
       <c r="G40" s="36"/>
     </row>
-    <row r="41" spans="2:33" s="20" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:33" s="20" customFormat="1" ht="30.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="38" t="s">
         <v>378</v>
       </c>
@@ -4336,7 +4336,7 @@
       </c>
       <c r="G41" s="36"/>
     </row>
-    <row r="42" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="77" t="s">
         <v>333</v>
       </c>
@@ -4346,7 +4346,7 @@
       </c>
       <c r="G42" s="36"/>
     </row>
-    <row r="43" spans="2:33" s="20" customFormat="1" ht="46.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:33" s="20" customFormat="1" ht="45.7" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B43" s="38" t="s">
         <v>303</v>
       </c>
@@ -4356,12 +4356,12 @@
       </c>
       <c r="G43" s="36"/>
     </row>
-    <row r="44" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="AG44" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B45" s="51"/>
       <c r="C45" s="51"/>
       <c r="D45" s="51"/>
@@ -4395,13 +4395,13 @@
       <c r="AF45" s="52"/>
       <c r="AG45" s="52"/>
     </row>
-    <row r="46" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:33" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B46" s="49"/>
       <c r="AG46" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:33" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:33" s="30" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B47" s="38" t="s">
         <v>379</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:33" s="20" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:33" s="20" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
       <c r="B48" s="58" t="s">
         <v>343</v>
       </c>
@@ -4424,7 +4424,7 @@
       <c r="E48" s="30"/>
       <c r="G48" s="36"/>
     </row>
-    <row r="49" spans="2:33" s="20" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:33" s="20" customFormat="1" ht="30.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" s="38" t="s">
         <v>344</v>
       </c>
@@ -4435,7 +4435,7 @@
       <c r="E49" s="30"/>
       <c r="G49" s="36"/>
     </row>
-    <row r="50" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" s="38" t="s">
         <v>359</v>
       </c>
@@ -4445,7 +4445,7 @@
       </c>
       <c r="G50" s="36"/>
     </row>
-    <row r="51" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" s="38" t="s">
         <v>361</v>
       </c>
@@ -4455,7 +4455,7 @@
       </c>
       <c r="G51" s="36"/>
     </row>
-    <row r="52" spans="2:33" s="20" customFormat="1" ht="47.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:33" s="20" customFormat="1" ht="31" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" s="38" t="s">
         <v>380</v>
       </c>
@@ -4465,7 +4465,7 @@
       </c>
       <c r="G52" s="36"/>
     </row>
-    <row r="53" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" s="81" t="s">
         <v>426</v>
       </c>
@@ -4475,7 +4475,7 @@
       </c>
       <c r="G53" s="36"/>
     </row>
-    <row r="54" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" s="77" t="s">
         <v>318</v>
       </c>
@@ -4484,7 +4484,7 @@
       </c>
       <c r="G54" s="36"/>
     </row>
-    <row r="55" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B55" s="77" t="s">
         <v>319</v>
       </c>
@@ -4493,7 +4493,7 @@
       </c>
       <c r="G55" s="36"/>
     </row>
-    <row r="56" spans="2:33" s="20" customFormat="1" ht="46.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:33" s="20" customFormat="1" ht="45.7" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B56" s="38" t="s">
         <v>370</v>
       </c>
@@ -4502,12 +4502,12 @@
       </c>
       <c r="G56" s="36"/>
     </row>
-    <row r="57" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:33" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B57" s="50"/>
       <c r="C57" s="50"/>
       <c r="D57" s="50"/>
     </row>
-    <row r="58" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:33" s="34" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B58" s="51"/>
       <c r="C58" s="51"/>
       <c r="D58" s="51"/>
@@ -4541,12 +4541,12 @@
       <c r="AF58" s="52"/>
       <c r="AG58" s="52"/>
     </row>
-    <row r="59" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="AG59" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B60" s="77" t="s">
         <v>381</v>
       </c>
@@ -4555,7 +4555,7 @@
       </c>
       <c r="G60" s="36"/>
     </row>
-    <row r="61" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B61" s="77" t="s">
         <v>382</v>
       </c>
@@ -4564,7 +4564,7 @@
       </c>
       <c r="G61" s="36"/>
     </row>
-    <row r="62" spans="2:33" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B62" s="38" t="s">
         <v>383</v>
       </c>
@@ -4573,7 +4573,7 @@
       </c>
       <c r="G62" s="36"/>
     </row>
-    <row r="63" spans="2:33" s="20" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:33" s="20" customFormat="1" ht="15.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B63" s="38" t="s">
         <v>384</v>
       </c>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="G63" s="36"/>
     </row>
-    <row r="64" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:33" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B64" s="77" t="s">
         <v>315</v>
       </c>
@@ -4591,7 +4591,7 @@
       </c>
       <c r="G64" s="36"/>
     </row>
-    <row r="65" spans="2:7" s="20" customFormat="1" ht="32.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:7" s="20" customFormat="1" ht="31" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B65" s="77" t="s">
         <v>397</v>
       </c>
@@ -4600,7 +4600,7 @@
       </c>
       <c r="G65" s="36"/>
     </row>
-    <row r="66" spans="2:7" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B66" s="77" t="s">
         <v>316</v>
       </c>
@@ -4609,7 +4609,7 @@
       </c>
       <c r="G66" s="36"/>
     </row>
-    <row r="67" spans="2:7" s="20" customFormat="1" ht="31.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" s="20" customFormat="1" ht="15.7" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B67" s="77" t="s">
         <v>398</v>
       </c>
@@ -4618,15 +4618,15 @@
       </c>
       <c r="G67" s="36"/>
     </row>
-    <row r="68" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.5">
       <c r="B68" s="50"/>
       <c r="D68" s="39"/>
     </row>
-    <row r="69" spans="2:7" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" s="40" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.5">
       <c r="G69" s="36"/>
     </row>
-    <row r="70" spans="2:7" s="40" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="2:7" s="20" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" s="40" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="71" spans="2:7" s="20" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
       <c r="B71" s="77" t="s">
         <v>385</v>
       </c>
@@ -4635,7 +4635,7 @@
       </c>
       <c r="G71" s="36"/>
     </row>
-    <row r="72" spans="2:7" s="20" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" s="20" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
       <c r="B72" s="77" t="s">
         <v>386</v>
       </c>
@@ -4644,7 +4644,7 @@
       </c>
       <c r="G72" s="36"/>
     </row>
-    <row r="73" spans="2:7" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B73" s="38" t="s">
         <v>425</v>
       </c>
@@ -4819,18 +4819,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.703125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="45.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.41015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5859375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="45.703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="21" t="s">
         <v>14</v>
       </c>
@@ -4838,7 +4838,7 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.5">
       <c r="G3" s="4"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -4852,7 +4852,7 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -4860,15 +4860,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B7" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B8" s="16"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -4876,7 +4876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B10" s="23" t="s">
         <v>20</v>
       </c>
@@ -4887,7 +4887,7 @@
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B11" s="23" t="s">
         <v>22</v>
       </c>
@@ -4898,7 +4898,7 @@
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B12" s="23" t="s">
         <v>24</v>
       </c>
@@ -4909,7 +4909,7 @@
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
     </row>
-    <row r="13" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B13" s="23" t="s">
         <v>26</v>
       </c>
@@ -4920,15 +4920,15 @@
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B14" s="20"/>
       <c r="C14" s="23"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B15" s="20"/>
       <c r="C15" s="23"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B16" s="16" t="s">
         <v>28</v>
       </c>
@@ -4945,7 +4945,7 @@
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.5">
       <c r="G17" s="4"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -4959,7 +4959,7 @@
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.5">
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -4990,7 +4990,7 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
     </row>
-    <row r="19" spans="2:18" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
       <c r="B19" s="20">
         <v>1</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B20" s="20">
         <v>2</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:18" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B21" s="20">
         <v>3</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B22" s="20">
         <v>4</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="2:18" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B23" s="20">
         <v>5</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B24" s="20">
         <v>6</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="2:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B25" s="20">
         <v>7</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="2:18" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
       <c r="B26" s="20">
         <v>8</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="2:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B27" s="20">
         <v>9</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B28" s="20">
         <v>10</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="2:18" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B29" s="20">
         <v>11</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="2:18" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B30" s="20">
         <v>12</v>
       </c>
@@ -5240,7 +5240,7 @@
       </c>
       <c r="G30" s="23"/>
     </row>
-    <row r="31" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B31" s="20">
         <v>13</v>
       </c>
@@ -5259,7 +5259,7 @@
       </c>
       <c r="G31" s="23"/>
     </row>
-    <row r="32" spans="2:18" s="20" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" s="20" customFormat="1" ht="157.69999999999999" x14ac:dyDescent="0.5">
       <c r="B32" s="20">
         <v>14</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B33" s="20">
         <v>15</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" s="20" customFormat="1" ht="86" x14ac:dyDescent="0.5">
       <c r="B34" s="20">
         <v>16</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B35" s="20">
         <v>17</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B36" s="20">
         <v>18</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
       <c r="B37" s="20">
         <v>19</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B38" s="20">
         <v>20</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B39" s="20">
         <v>21</v>
       </c>
@@ -5425,7 +5425,7 @@
       </c>
       <c r="G39" s="23"/>
     </row>
-    <row r="40" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B40" s="20">
         <v>22</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B41" s="20">
         <v>23</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B42" s="20">
         <v>24</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
       <c r="B43" s="20">
         <v>25</v>
       </c>
@@ -5509,7 +5509,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="2:7" s="20" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" s="20" customFormat="1" ht="114.7" x14ac:dyDescent="0.5">
       <c r="B44" s="20">
         <v>26</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B45" s="20">
         <v>27</v>
       </c>
@@ -5549,7 +5549,7 @@
       </c>
       <c r="G45" s="23"/>
     </row>
-    <row r="46" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B46" s="20">
         <v>28</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="2:7" s="20" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" s="20" customFormat="1" ht="114.7" x14ac:dyDescent="0.5">
       <c r="B47" s="20">
         <v>29</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B48" s="20">
         <v>30</v>
       </c>
@@ -5610,7 +5610,7 @@
       </c>
       <c r="G48" s="23"/>
     </row>
-    <row r="49" spans="2:12" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
       <c r="B49" s="20">
         <v>31</v>
       </c>
@@ -5629,7 +5629,7 @@
       </c>
       <c r="G49" s="23"/>
     </row>
-    <row r="50" spans="2:12" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B50" s="20">
         <v>32</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:12" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B51" s="20">
         <v>33</v>
       </c>
@@ -5669,7 +5669,7 @@
       </c>
       <c r="G51" s="23"/>
     </row>
-    <row r="52" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B52" s="20">
         <v>34</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B53" s="20">
         <v>35</v>
       </c>
@@ -5709,7 +5709,7 @@
       </c>
       <c r="G53" s="23"/>
     </row>
-    <row r="54" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B54" s="20">
         <v>36</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B55" s="20">
         <v>37</v>
       </c>
@@ -5749,7 +5749,7 @@
       </c>
       <c r="G55" s="23"/>
     </row>
-    <row r="56" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B56" s="20">
         <v>38</v>
       </c>
@@ -5765,7 +5765,7 @@
       </c>
       <c r="G56" s="23"/>
     </row>
-    <row r="57" spans="2:12" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" s="20">
         <v>39</v>
       </c>
@@ -5785,7 +5785,7 @@
       <c r="G57" s="23"/>
       <c r="L57" s="27"/>
     </row>
-    <row r="58" spans="2:12" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B58" s="20">
         <v>40</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B59" s="20">
         <v>41</v>
       </c>
@@ -5827,7 +5827,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B60" s="20">
         <v>42</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="2:12" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B61" s="20">
         <v>43</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B62" s="20">
         <v>44</v>
       </c>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="G62" s="23"/>
     </row>
-    <row r="63" spans="2:12" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B63" s="20">
         <v>45</v>
       </c>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="G63" s="23"/>
     </row>
-    <row r="64" spans="2:12" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:12" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B64" s="20">
         <v>46</v>
       </c>
@@ -5926,7 +5926,7 @@
       </c>
       <c r="G64" s="23"/>
     </row>
-    <row r="65" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B65" s="20">
         <v>47</v>
       </c>
@@ -5945,7 +5945,7 @@
       </c>
       <c r="G65" s="23"/>
     </row>
-    <row r="66" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B66" s="20">
         <v>48</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B67" s="20">
         <v>49</v>
       </c>
@@ -5985,7 +5985,7 @@
       </c>
       <c r="G67" s="23"/>
     </row>
-    <row r="68" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B68" s="20">
         <v>50</v>
       </c>
@@ -6004,7 +6004,7 @@
       </c>
       <c r="G68" s="23"/>
     </row>
-    <row r="69" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B69" s="20">
         <v>51</v>
       </c>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="G69" s="23"/>
     </row>
-    <row r="70" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B70" s="20">
         <v>52</v>
       </c>
@@ -6042,7 +6042,7 @@
       </c>
       <c r="G70" s="23"/>
     </row>
-    <row r="71" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B71" s="20">
         <v>53</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="2:7" s="20" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" s="20" customFormat="1" ht="114.7" x14ac:dyDescent="0.5">
       <c r="B72" s="20">
         <v>54</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B73" s="20">
         <v>55</v>
       </c>
@@ -6105,7 +6105,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B74" s="20">
         <v>56</v>
       </c>
@@ -6126,7 +6126,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="75" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B75" s="20">
         <v>57</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B76" s="20">
         <v>58</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="77" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
       <c r="B77" s="20">
         <v>59</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="78" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B78" s="20">
         <v>60</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B79" s="20">
         <v>61</v>
       </c>
@@ -6231,7 +6231,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="80" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B80" s="20">
         <v>62</v>
       </c>
@@ -6250,7 +6250,7 @@
       </c>
       <c r="G80" s="23"/>
     </row>
-    <row r="81" spans="2:7" s="20" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" s="20" customFormat="1" ht="172" x14ac:dyDescent="0.5">
       <c r="B81" s="20">
         <v>63</v>
       </c>
@@ -6271,7 +6271,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B82" s="20">
         <v>64</v>
       </c>
@@ -6292,7 +6292,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="83" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B83" s="20">
         <v>65</v>
       </c>
@@ -6311,7 +6311,7 @@
       </c>
       <c r="G83" s="23"/>
     </row>
-    <row r="84" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" ht="43" x14ac:dyDescent="0.5">
       <c r="B84" s="20">
         <v>66</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B85" s="20">
         <v>67</v>
       </c>
@@ -6351,7 +6351,7 @@
       </c>
       <c r="G85" s="23"/>
     </row>
-    <row r="86" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B86" s="20">
         <v>68</v>
       </c>
@@ -6372,7 +6372,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="87" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
       <c r="B87" s="20">
         <v>69</v>
       </c>
@@ -6393,7 +6393,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="88" spans="2:7" s="20" customFormat="1" ht="285" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" s="20" customFormat="1" ht="229.35" x14ac:dyDescent="0.5">
       <c r="B88" s="20">
         <v>70</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="89" spans="2:7" s="20" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" s="20" customFormat="1" ht="258" x14ac:dyDescent="0.5">
       <c r="B89" s="20" t="s">
         <v>336</v>
       </c>
@@ -6435,7 +6435,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="90" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B90" s="20" t="s">
         <v>339</v>
       </c>
@@ -6456,7 +6456,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="91" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B91" s="20" t="s">
         <v>342</v>
       </c>
@@ -6475,7 +6475,7 @@
       </c>
       <c r="G91" s="59"/>
     </row>
-    <row r="92" spans="2:7" s="20" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" s="20" customFormat="1" ht="186.35" x14ac:dyDescent="0.5">
       <c r="B92" s="20">
         <v>71</v>
       </c>
@@ -6496,7 +6496,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="93" spans="2:7" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7" s="20" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B93" s="20">
         <v>71</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="94" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
       <c r="B94" s="20">
         <v>72</v>
       </c>
@@ -6538,7 +6538,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="95" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B95" s="20">
         <v>73</v>
       </c>
@@ -6557,7 +6557,7 @@
       </c>
       <c r="G95" s="23"/>
     </row>
-    <row r="96" spans="2:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:7" s="20" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
       <c r="B96" s="20">
         <v>74</v>
       </c>
@@ -6578,7 +6578,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="97" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B97" s="20">
         <v>75</v>
       </c>
@@ -6597,7 +6597,7 @@
       </c>
       <c r="G97" s="23"/>
     </row>
-    <row r="98" spans="2:7" s="20" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7" s="20" customFormat="1" ht="129" x14ac:dyDescent="0.5">
       <c r="B98" s="20">
         <v>76</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="99" spans="2:7" s="20" customFormat="1" ht="390" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" s="20" customFormat="1" ht="329.7" x14ac:dyDescent="0.5">
       <c r="B99" s="20">
         <v>77</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="100" spans="2:7" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
       <c r="B100" s="20">
         <v>78</v>
       </c>
@@ -6660,7 +6660,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="101" spans="2:7" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
       <c r="B101" s="20">
         <v>79</v>
       </c>
@@ -6681,7 +6681,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="102" spans="2:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:7" s="20" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B102" s="20">
         <v>80</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="103" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:7" s="20" customFormat="1" ht="86" x14ac:dyDescent="0.5">
       <c r="B103" s="20">
         <v>81</v>
       </c>
@@ -6723,7 +6723,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="104" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:7" s="20" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B104" s="20">
         <v>82</v>
       </c>
@@ -6742,7 +6742,7 @@
       </c>
       <c r="G104" s="23"/>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B105" s="20">
         <v>83</v>
       </c>
@@ -6761,7 +6761,7 @@
       </c>
       <c r="G105" s="23"/>
     </row>
-    <row r="106" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:7" ht="71.7" x14ac:dyDescent="0.5">
       <c r="B106" s="20">
         <v>84</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="107" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:7" ht="43" x14ac:dyDescent="0.5">
       <c r="B107" s="20">
         <v>85</v>
       </c>
@@ -6801,7 +6801,7 @@
       </c>
       <c r="G107" s="23"/>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B108" s="20">
         <v>86</v>
       </c>
@@ -6820,7 +6820,7 @@
       </c>
       <c r="G108" s="23"/>
     </row>
-    <row r="109" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B109" s="20">
         <v>87</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="110" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B110" s="20">
         <v>88</v>
       </c>
@@ -6860,7 +6860,7 @@
       </c>
       <c r="G110" s="23"/>
     </row>
-    <row r="111" spans="2:7" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:7" s="20" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
       <c r="B111" s="20">
         <v>89</v>
       </c>
@@ -6881,7 +6881,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="112" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B112" s="20">
         <v>90</v>
       </c>
@@ -6900,7 +6900,7 @@
       </c>
       <c r="G112" s="23"/>
     </row>
-    <row r="113" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B113" s="20">
         <v>91</v>
       </c>
@@ -6919,7 +6919,7 @@
       </c>
       <c r="G113" s="23"/>
     </row>
-    <row r="114" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:7" ht="43" x14ac:dyDescent="0.5">
       <c r="B114" s="20">
         <v>92</v>
       </c>
@@ -6938,7 +6938,7 @@
       </c>
       <c r="G114" s="23"/>
     </row>
-    <row r="115" spans="2:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:7" ht="129" x14ac:dyDescent="0.5">
       <c r="B115" s="20">
         <v>93</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B116" s="20">
         <v>94</v>
       </c>
@@ -6969,7 +6969,7 @@
       <c r="F116" s="23"/>
       <c r="G116" s="23"/>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B117" s="20">
         <v>95</v>
       </c>
@@ -6979,7 +6979,7 @@
       <c r="F117" s="23"/>
       <c r="G117" s="23"/>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B118" s="20">
         <v>96</v>
       </c>
@@ -6989,7 +6989,7 @@
       <c r="F118" s="23"/>
       <c r="G118" s="23"/>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B119" s="20">
         <v>97</v>
       </c>
@@ -6999,7 +6999,7 @@
       <c r="F119" s="23"/>
       <c r="G119" s="23"/>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B120" s="20">
         <v>98</v>
       </c>
@@ -7009,7 +7009,7 @@
       <c r="F120" s="23"/>
       <c r="G120" s="23"/>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B121" s="20">
         <v>99</v>
       </c>
@@ -7019,7 +7019,7 @@
       <c r="F121" s="23"/>
       <c r="G121" s="23"/>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B122" s="20">
         <v>100</v>
       </c>
@@ -7053,21 +7053,21 @@
       <selection activeCell="B218" sqref="B218"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="92.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" customWidth="1"/>
-    <col min="4" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="17" width="16.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="3.703125" customWidth="1"/>
+    <col min="2" max="2" width="92.29296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.1171875" customWidth="1"/>
+    <col min="4" max="5" width="16.703125" customWidth="1"/>
+    <col min="6" max="17" width="16.703125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" s="71" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" s="71" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="71" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -7087,7 +7087,7 @@
       <c r="P4"/>
       <c r="Q4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -7106,7 +7106,7 @@
       <c r="P5"/>
       <c r="Q5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -7125,7 +7125,7 @@
       <c r="P6"/>
       <c r="Q6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
       <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -7138,12 +7138,12 @@
       <c r="P7"/>
       <c r="Q7"/>
     </row>
-    <row r="8" spans="1:17" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B8" s="72" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.5">
       <c r="G9"/>
       <c r="H9"/>
       <c r="I9"/>
@@ -7156,7 +7156,7 @@
       <c r="P9"/>
       <c r="Q9"/>
     </row>
-    <row r="10" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B10" s="16" t="s">
         <v>187</v>
       </c>
@@ -7178,7 +7178,7 @@
       <c r="P10" s="73"/>
       <c r="Q10" s="73"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B11" t="s">
         <v>190</v>
       </c>
@@ -7192,7 +7192,7 @@
       </c>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
         <v>192</v>
       </c>
@@ -7206,7 +7206,7 @@
       </c>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B13" t="s">
         <v>191</v>
       </c>
@@ -7220,80 +7220,80 @@
       </c>
       <c r="G13"/>
     </row>
-    <row r="15" spans="1:17" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B15" s="72" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B17" s="16" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B19" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B22" s="16" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B23" s="16"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B24" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B25" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B26" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B28" s="16" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B30" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B31" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B32" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B33" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B35" s="16" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B37" t="str">
         <f t="shared" ref="B37:B43" si="0">D38</f>
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
@@ -7312,7 +7312,7 @@
       <c r="P37"/>
       <c r="Q37"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>Gas Control Device/Control System Component</v>
@@ -7331,7 +7331,7 @@
       <c r="P38"/>
       <c r="Q38"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B39" t="str">
         <f t="shared" si="0"/>
         <v>Landfill Surface: Daily Cover</v>
@@ -7349,7 +7349,7 @@
       <c r="P39"/>
       <c r="Q39"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>Landfill Surface: Final Cover</v>
@@ -7367,7 +7367,7 @@
       <c r="P40"/>
       <c r="Q40"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>Landfill Surface: Intermediate Cover</v>
@@ -7385,7 +7385,7 @@
       <c r="P41"/>
       <c r="Q41"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>Leachate Management System</v>
@@ -7403,7 +7403,7 @@
       <c r="P42"/>
       <c r="Q42"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
@@ -7421,25 +7421,25 @@
       <c r="P43"/>
       <c r="Q43"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.5">
       <c r="D44" s="7" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B45" s="16" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B46" s="16"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B47" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="48" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B48" s="67" t="str" cm="1">
         <f t="array" ref="B48:B58">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn.TOCOL(C64:M70, 1)))</f>
         <v>Collection system downtime</v>
@@ -7447,89 +7447,89 @@
       <c r="E48" s="7"/>
       <c r="Q48"/>
     </row>
-    <row r="49" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B49" s="69" t="str">
         <v>Construction - New Well Installation</v>
       </c>
       <c r="E49" s="7"/>
       <c r="Q49"/>
     </row>
-    <row r="50" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B50" s="70" t="str">
         <v>Construction - Well Raising or Horizontal Extension</v>
       </c>
       <c r="E50" s="7"/>
       <c r="Q50"/>
     </row>
-    <row r="51" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B51" s="68" t="str">
         <v>Cover integrity</v>
       </c>
       <c r="E51" s="7"/>
       <c r="Q51"/>
     </row>
-    <row r="52" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B52" s="67" t="str">
         <v>Cover-related Construction (Excavation/ Exposed Operations/ Re-grading)</v>
       </c>
       <c r="E52" s="7"/>
       <c r="Q52"/>
     </row>
-    <row r="53" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B53" s="68" t="str">
         <v>Cracked/Broken Seal</v>
       </c>
       <c r="E53" s="7"/>
       <c r="Q53"/>
     </row>
-    <row r="54" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B54" s="67" t="str">
         <v>Damaged component</v>
       </c>
       <c r="E54" s="7"/>
       <c r="Q54"/>
     </row>
-    <row r="55" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B55" s="67" t="str">
         <v>Insufficient vacuum</v>
       </c>
       <c r="E55" s="7"/>
       <c r="Q55"/>
     </row>
-    <row r="56" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B56" s="69" t="str">
         <v>Offline Gas Collection Well(s)</v>
       </c>
       <c r="E56" s="7"/>
       <c r="Q56"/>
     </row>
-    <row r="57" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B57" s="70" t="str">
         <v>Other</v>
       </c>
       <c r="E57" s="7"/>
       <c r="Q57"/>
     </row>
-    <row r="58" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B58" s="68" t="str">
         <v>Uncontrolled Area (no gas collection infrastructure)</v>
       </c>
       <c r="E58" s="7"/>
       <c r="Q58"/>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B60" s="16" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.5">
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="12" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:17" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B62" s="3" t="s">
         <v>176</v>
       </c>
@@ -7537,7 +7537,7 @@
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:17" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="B63" s="2" t="s">
         <v>177</v>
       </c>
@@ -7547,7 +7547,7 @@
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="2:17" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:17" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B64" s="6" t="s">
         <v>399</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B65" s="10" t="s">
         <v>167</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="66" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B66" s="10" t="s">
         <v>168</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="67" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B67" s="6" t="s">
         <v>169</v>
       </c>
@@ -7687,7 +7687,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="68" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B68" s="10" t="s">
         <v>170</v>
       </c>
@@ -7711,7 +7711,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="69" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B69" s="10" t="s">
         <v>186</v>
       </c>
@@ -7741,7 +7741,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="70" spans="2:13" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:13" ht="59.7" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B70" s="6" t="s">
         <v>13</v>
       </c>
@@ -7763,12 +7763,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B72" s="16" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B74" t="str" cm="1">
         <f t="array" ref="B74:C125">_xlfn.HSTACK(_xlfn.TOCOL(_xlfn.IFS(C64:M70&lt;&gt;"",B64:B70),3),_xlfn.TOCOL(C64:M70,1))</f>
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
@@ -7778,7 +7778,7 @@
       </c>
       <c r="G74"/>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B75" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7787,7 +7787,7 @@
       </c>
       <c r="G75"/>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B76" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7796,7 +7796,7 @@
       </c>
       <c r="G76"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B77" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7805,7 +7805,7 @@
       </c>
       <c r="G77"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B78" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7814,7 +7814,7 @@
       </c>
       <c r="G78"/>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B79" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
@@ -7823,7 +7823,7 @@
       </c>
       <c r="G79"/>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B80" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7832,7 +7832,7 @@
       </c>
       <c r="G80"/>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B81" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7841,7 +7841,7 @@
       </c>
       <c r="G81"/>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B82" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7850,7 +7850,7 @@
       </c>
       <c r="G82"/>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B83" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7859,7 +7859,7 @@
       </c>
       <c r="G83"/>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B84" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7868,7 +7868,7 @@
       </c>
       <c r="G84"/>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B85" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7877,7 +7877,7 @@
       </c>
       <c r="G85"/>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B86" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7886,7 +7886,7 @@
       </c>
       <c r="G86"/>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B87" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7895,7 +7895,7 @@
       </c>
       <c r="G87"/>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B88" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7904,7 +7904,7 @@
       </c>
       <c r="G88"/>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B89" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7913,7 +7913,7 @@
       </c>
       <c r="G89"/>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B90" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -7922,7 +7922,7 @@
       </c>
       <c r="G90"/>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B91" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7931,7 +7931,7 @@
       </c>
       <c r="G91"/>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B92" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7940,7 +7940,7 @@
       </c>
       <c r="G92"/>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B93" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7949,7 +7949,7 @@
       </c>
       <c r="G93"/>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B94" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7958,7 +7958,7 @@
       </c>
       <c r="G94"/>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B95" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7967,7 +7967,7 @@
       </c>
       <c r="G95"/>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B96" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7976,7 +7976,7 @@
       </c>
       <c r="G96"/>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B97" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7985,7 +7985,7 @@
       </c>
       <c r="G97"/>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B98" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -7994,7 +7994,7 @@
       </c>
       <c r="G98"/>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B99" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8003,7 +8003,7 @@
       </c>
       <c r="G99"/>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B100" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8012,7 +8012,7 @@
       </c>
       <c r="G100"/>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B101" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8021,7 +8021,7 @@
       </c>
       <c r="G101"/>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B102" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8030,7 +8030,7 @@
       </c>
       <c r="G102"/>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B103" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8039,7 +8039,7 @@
       </c>
       <c r="G103"/>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B104" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8048,7 +8048,7 @@
       </c>
       <c r="G104"/>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B105" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8057,7 +8057,7 @@
       </c>
       <c r="G105"/>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B106" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8066,7 +8066,7 @@
       </c>
       <c r="G106"/>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B107" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8075,7 +8075,7 @@
       </c>
       <c r="G107"/>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B108" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8084,7 +8084,7 @@
       </c>
       <c r="G108"/>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B109" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8093,7 +8093,7 @@
       </c>
       <c r="G109"/>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B110" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8102,7 +8102,7 @@
       </c>
       <c r="G110"/>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B111" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8111,7 +8111,7 @@
       </c>
       <c r="G111"/>
     </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B112" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8120,7 +8120,7 @@
       </c>
       <c r="G112"/>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B113" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8129,7 +8129,7 @@
       </c>
       <c r="G113"/>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B114" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8138,7 +8138,7 @@
       </c>
       <c r="G114"/>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B115" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8147,7 +8147,7 @@
       </c>
       <c r="G115"/>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B116" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8156,7 +8156,7 @@
       </c>
       <c r="G116"/>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B117" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8165,7 +8165,7 @@
       </c>
       <c r="G117"/>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B118" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8174,7 +8174,7 @@
       </c>
       <c r="G118"/>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B119" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8183,7 +8183,7 @@
       </c>
       <c r="G119"/>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B120" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8192,7 +8192,7 @@
       </c>
       <c r="G120"/>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B121" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8201,7 +8201,7 @@
       </c>
       <c r="G121"/>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B122" t="str">
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
       </c>
@@ -8210,7 +8210,7 @@
       </c>
       <c r="G122"/>
     </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B123" t="str">
         <v>Gas Control Device/Control System Component</v>
       </c>
@@ -8218,7 +8218,7 @@
         <v>Cover-related Construction (Excavation/ Exposed Operations/ Re-grading)</v>
       </c>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B124" t="str">
         <v>Gas Control Device/Control System Component</v>
       </c>
@@ -8227,7 +8227,7 @@
       </c>
       <c r="G124"/>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B125" t="str">
         <v>Gas Control Device/Control System Component</v>
       </c>
@@ -8236,21 +8236,21 @@
       </c>
       <c r="G125"/>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G126"/>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G134"/>
     </row>
-    <row r="135" spans="2:7" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B135" s="72" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G136"/>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B137" s="17" t="s">
         <v>193</v>
       </c>
@@ -8259,12 +8259,12 @@
       </c>
       <c r="G137"/>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B138" s="16"/>
       <c r="C138" s="16"/>
       <c r="G138"/>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B139" t="s">
         <v>163</v>
       </c>
@@ -8274,7 +8274,7 @@
       </c>
       <c r="G139"/>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B140" t="str" cm="1">
         <f t="array" ref="B140:B142">_carb_only_table_02[]</f>
         <v>Operator was aware of the leak prior to receiving the CARB plume notification</v>
@@ -8284,7 +8284,7 @@
       </c>
       <c r="G140"/>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B141" t="str">
         <v>Operator detected a leak during follow-up monitoring after receipt of the CARB plume notification</v>
       </c>
@@ -8293,7 +8293,7 @@
       </c>
       <c r="G141"/>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B142" t="str">
         <v>No leak was detected</v>
       </c>
@@ -8302,18 +8302,18 @@
       </c>
       <c r="G142"/>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G143"/>
     </row>
-    <row r="144" spans="2:7" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B144" s="72" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G145"/>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B146" s="17" t="s">
         <v>193</v>
       </c>
@@ -8322,12 +8322,12 @@
       </c>
       <c r="G146"/>
     </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B147" s="16"/>
       <c r="C147" s="16"/>
       <c r="G147"/>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B148" t="s">
         <v>163</v>
       </c>
@@ -8337,7 +8337,7 @@
       </c>
       <c r="G148"/>
     </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B149" t="str">
         <f ca="1">IF(C11=B26, "Not applicable as no leak was detected", "")</f>
         <v/>
@@ -8348,7 +8348,7 @@
       </c>
       <c r="G149"/>
     </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B150" t="str" cm="1">
         <f t="array" ref="B150:B153">_carb_only_table_03[]</f>
         <v>Operator was aware of the leak prior to receiving the notification, and/or repairs were in progress on the date of the plume observation</v>
@@ -8359,7 +8359,7 @@
       </c>
       <c r="G150"/>
     </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B151" t="str">
         <v>An unintentional leak  (i.e., the operator was not aware of, and could be repaired if discovered)</v>
       </c>
@@ -8369,7 +8369,7 @@
       </c>
       <c r="G151"/>
     </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B152" t="str">
         <v>An intentional or allowable vent (i.e., the operator was aware of, and/or would not repair)</v>
       </c>
@@ -8379,24 +8379,24 @@
       </c>
       <c r="G152"/>
     </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B153" t="str">
         <v>Due to a temporary activity (i.e., would be resolved without corrective action when the activity is complete)</v>
       </c>
       <c r="G153"/>
     </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G154"/>
     </row>
-    <row r="155" spans="2:7" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B155" s="72" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G156"/>
     </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B157" s="17" t="s">
         <v>193</v>
       </c>
@@ -8405,12 +8405,12 @@
       </c>
       <c r="G157"/>
     </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B158" s="16"/>
       <c r="C158" s="16"/>
       <c r="G158"/>
     </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B159" t="s">
         <v>163</v>
       </c>
@@ -8420,7 +8420,7 @@
       </c>
       <c r="G159"/>
     </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B160" t="str">
         <f ca="1">IF(C11=B26, "Not applicable as no leak was detected", "")</f>
         <v/>
@@ -8431,7 +8431,7 @@
       </c>
       <c r="G160"/>
     </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B161" t="str" cm="1">
         <f t="array" ref="B161:B167">_carb_only_table_04[]</f>
         <v>Gas Collection System Component (e.g., blower, well, valve, port)</v>
@@ -8442,7 +8442,7 @@
       </c>
       <c r="G161"/>
     </row>
-    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B162" t="str">
         <v>Gas Control Device/Control System Component</v>
       </c>
@@ -8452,7 +8452,7 @@
       </c>
       <c r="G162"/>
     </row>
-    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B163" t="str">
         <v>Landfill Surface: Daily Cover</v>
       </c>
@@ -8462,7 +8462,7 @@
       </c>
       <c r="G163"/>
     </row>
-    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B164" t="str">
         <v>Landfill Surface: Final Cover</v>
       </c>
@@ -8472,7 +8472,7 @@
       </c>
       <c r="G164"/>
     </row>
-    <row r="165" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B165" t="str">
         <v>Landfill Surface: Intermediate Cover</v>
       </c>
@@ -8482,7 +8482,7 @@
       </c>
       <c r="G165"/>
     </row>
-    <row r="166" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B166" t="str">
         <v>Leachate Management System</v>
       </c>
@@ -8492,24 +8492,24 @@
       </c>
       <c r="G166"/>
     </row>
-    <row r="167" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B167" t="str">
         <v>Working Face (area where active filling was being conducted at the time of detection)</v>
       </c>
       <c r="G167"/>
     </row>
-    <row r="168" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G168"/>
     </row>
-    <row r="169" spans="2:7" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B169" s="72" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="170" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G170"/>
     </row>
-    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B171" s="17" t="s">
         <v>193</v>
       </c>
@@ -8518,12 +8518,12 @@
       </c>
       <c r="G171"/>
     </row>
-    <row r="172" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B172" s="16"/>
       <c r="C172" s="16"/>
       <c r="G172"/>
     </row>
-    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B173" t="s">
         <v>163</v>
       </c>
@@ -8533,74 +8533,74 @@
       </c>
       <c r="G173"/>
     </row>
-    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B174" t="str">
         <f ca="1">IF(C11=B26, "Not applicable as no leak was detected", "")</f>
         <v/>
       </c>
       <c r="G174"/>
     </row>
-    <row r="175" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B175" t="str" cm="1">
         <f t="array" aca="1" ref="B175" ca="1">_xlfn._xlws.FILTER($C$74:$C$125, $B$74:$B$125=C13, "")</f>
         <v/>
       </c>
       <c r="G175"/>
     </row>
-    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G176"/>
     </row>
-    <row r="177" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G177"/>
     </row>
-    <row r="178" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G178"/>
     </row>
-    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G179"/>
     </row>
-    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G180"/>
     </row>
-    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G181"/>
     </row>
-    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G182"/>
     </row>
-    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G183"/>
     </row>
-    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G184"/>
     </row>
-    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G185"/>
     </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G186"/>
     </row>
-    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G187"/>
     </row>
-    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G188"/>
     </row>
-    <row r="189" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G189"/>
     </row>
-    <row r="190" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G190"/>
     </row>
-    <row r="191" spans="2:7" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B191" s="72" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="192" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G192"/>
     </row>
-    <row r="193" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B193" s="17" t="s">
         <v>193</v>
       </c>
@@ -8609,12 +8609,12 @@
       </c>
       <c r="G193"/>
     </row>
-    <row r="194" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B194" s="16"/>
       <c r="C194" s="16"/>
       <c r="G194"/>
     </row>
-    <row r="195" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B195" t="s">
         <v>163</v>
       </c>
@@ -8624,7 +8624,7 @@
       </c>
       <c r="G195"/>
     </row>
-    <row r="196" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B196" t="str">
         <f ca="1">IF(C11=B26, "Not applicable as no leak was detected", "")</f>
         <v/>
@@ -8635,65 +8635,65 @@
       </c>
       <c r="G196"/>
     </row>
-    <row r="197" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B197" t="s">
         <v>355</v>
       </c>
       <c r="G197"/>
     </row>
-    <row r="198" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B198" t="str" cm="1">
         <f t="array" aca="1" ref="B198" ca="1">_xlfn._xlws.FILTER($C$74:$C$125, $B$74:$B$125=C13, "")</f>
         <v/>
       </c>
       <c r="G198"/>
     </row>
-    <row r="199" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G199"/>
     </row>
-    <row r="200" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G200"/>
     </row>
-    <row r="201" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G201"/>
     </row>
-    <row r="202" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G202"/>
     </row>
-    <row r="203" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G203"/>
     </row>
-    <row r="204" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G204"/>
     </row>
-    <row r="205" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G205"/>
     </row>
-    <row r="206" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G206"/>
     </row>
-    <row r="207" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G207"/>
     </row>
-    <row r="208" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G208"/>
     </row>
-    <row r="209" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G209"/>
     </row>
-    <row r="210" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:7" x14ac:dyDescent="0.5">
       <c r="G210"/>
     </row>
-    <row r="213" spans="2:7" s="72" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:7" s="72" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B213" s="72" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="214" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B214" s="16"/>
       <c r="G214"/>
     </row>
-    <row r="215" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B215" s="17" t="s">
         <v>193</v>
       </c>
@@ -8702,12 +8702,12 @@
       </c>
       <c r="G215"/>
     </row>
-    <row r="216" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B216" s="16"/>
       <c r="C216" s="16"/>
       <c r="G216"/>
     </row>
-    <row r="217" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B217" t="s">
         <v>163</v>
       </c>
@@ -8717,7 +8717,7 @@
       </c>
       <c r="G217"/>
     </row>
-    <row r="218" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B218" t="str" cm="1">
         <f t="array" ref="B218:B219">_carb_only_table_01[]</f>
         <v>Yes</v>
@@ -8727,7 +8727,7 @@
       </c>
       <c r="G218"/>
     </row>
-    <row r="219" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B219" t="str">
         <v>No</v>
       </c>
@@ -8755,19 +8755,19 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="9" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.703125" customWidth="1"/>
+    <col min="2" max="3" width="30.703125" customWidth="1"/>
+    <col min="4" max="9" width="8.703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" s="14" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="14" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -8775,7 +8775,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -8783,7 +8783,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -8791,7 +8791,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -8799,7 +8799,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="15" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="15" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B14" s="15" t="s">
         <v>200</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>202</v>
       </c>
@@ -8829,18 +8829,18 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="3" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.703125" customWidth="1"/>
+    <col min="2" max="3" width="30.703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" s="14" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="14" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -8848,7 +8848,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -8856,7 +8856,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -8864,7 +8864,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -8872,12 +8872,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" s="15" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="10" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="12" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="13" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:3" s="15" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B14" s="15" t="s">
         <v>206</v>
       </c>
@@ -8885,7 +8885,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>208</v>
       </c>
@@ -8893,7 +8893,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
         <v>210</v>
       </c>
@@ -8912,28 +8912,28 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.703125" customWidth="1"/>
+    <col min="2" max="2" width="25.1171875" customWidth="1"/>
+    <col min="3" max="3" width="16.41015625" customWidth="1"/>
+    <col min="4" max="4" width="32.41015625" customWidth="1"/>
+    <col min="5" max="5" width="16.41015625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="99" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="21" t="s">
         <v>212</v>
       </c>
       <c r="C2" s="22"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -8943,26 +8943,26 @@
       <c r="C4" s="1"/>
       <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="C5" s="1"/>
       <c r="F5" s="19"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="C6" s="1"/>
       <c r="F6" s="19"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="C7" s="1"/>
       <c r="F7" s="19"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="C8" s="1"/>
       <c r="F8" s="19"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F9" s="19"/>
     </row>
-    <row r="10" spans="1:6" s="15" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" s="15" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B10" s="15" t="s">
         <v>200</v>
       </c>
@@ -8979,7 +8979,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B11" t="s">
         <v>350</v>
       </c>
@@ -8996,7 +8996,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
         <v>350</v>
       </c>
@@ -9013,321 +9013,321 @@
         <v>399</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B13" t="s">
         <v>202</v>
       </c>
       <c r="C13" t="s">
-        <v>400</v>
+        <v>242</v>
       </c>
       <c r="D13" t="s">
-        <v>217</v>
+        <v>240</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B14" t="s">
         <v>202</v>
       </c>
       <c r="C14" t="s">
-        <v>401</v>
+        <v>270</v>
       </c>
       <c r="D14" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
       </c>
-      <c r="F14" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>202</v>
       </c>
       <c r="C15" t="s">
-        <v>402</v>
+        <v>257</v>
       </c>
       <c r="D15" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
       </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="28">
+        <v>45468</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
         <v>202</v>
       </c>
       <c r="C16" t="s">
-        <v>220</v>
+        <v>261</v>
       </c>
       <c r="D16" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
       </c>
-      <c r="F16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>35.321100000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B17" t="s">
         <v>202</v>
       </c>
       <c r="C17" t="s">
-        <v>222</v>
+        <v>269</v>
       </c>
       <c r="D17" t="s">
-        <v>223</v>
+        <v>262</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
       </c>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>-119.5808</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B18" t="s">
         <v>202</v>
       </c>
       <c r="C18" t="s">
-        <v>232</v>
+        <v>404</v>
       </c>
       <c r="D18" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="E18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B19" t="s">
         <v>202</v>
       </c>
       <c r="C19" t="s">
-        <v>403</v>
+        <v>236</v>
       </c>
       <c r="D19" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B20" t="s">
         <v>202</v>
       </c>
       <c r="C20" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="D20" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="E20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B21" t="s">
         <v>202</v>
       </c>
       <c r="C21" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D21" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="E21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B22" t="s">
         <v>202</v>
       </c>
       <c r="C22" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="D22" t="s">
-        <v>190</v>
+        <v>223</v>
       </c>
       <c r="E22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B23" t="s">
         <v>202</v>
       </c>
       <c r="C23" t="s">
-        <v>235</v>
+        <v>402</v>
       </c>
       <c r="D23" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="E23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B24" t="s">
         <v>202</v>
       </c>
       <c r="C24" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="D24" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
       </c>
-      <c r="F24" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="28">
+        <v>45152</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B25" t="s">
         <v>202</v>
       </c>
       <c r="C25" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="D25" t="s">
-        <v>192</v>
+        <v>253</v>
       </c>
       <c r="E25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B26" t="s">
         <v>202</v>
       </c>
       <c r="C26" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D26" t="s">
-        <v>237</v>
+        <v>190</v>
       </c>
       <c r="E26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B27" t="s">
         <v>202</v>
       </c>
       <c r="C27" t="s">
-        <v>238</v>
+        <v>400</v>
       </c>
       <c r="D27" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B28" t="s">
         <v>202</v>
       </c>
       <c r="C28" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="D28" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B29" t="s">
         <v>202</v>
       </c>
       <c r="C29" t="s">
-        <v>404</v>
+        <v>259</v>
       </c>
       <c r="D29" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
       </c>
-      <c r="F29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>35.321100000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B30" t="s">
         <v>202</v>
       </c>
       <c r="C30" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D30" t="s">
-        <v>243</v>
+        <v>264</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+        <v>-119.5808</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B31" t="s">
         <v>202</v>
       </c>
       <c r="C31" t="s">
-        <v>274</v>
+        <v>234</v>
       </c>
       <c r="D31" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
@@ -9336,299 +9336,299 @@
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B32" t="s">
         <v>202</v>
       </c>
       <c r="C32" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="D32" t="s">
-        <v>247</v>
+        <v>191</v>
       </c>
       <c r="E32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B33" t="s">
         <v>202</v>
       </c>
       <c r="C33" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="D33" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
       </c>
-      <c r="F33">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B34" t="s">
         <v>202</v>
       </c>
       <c r="C34" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="D34" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="E34" t="b">
-        <v>0</v>
-      </c>
-      <c r="F34" s="28">
-        <v>45152</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B35" t="s">
         <v>202</v>
       </c>
       <c r="C35" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="D35" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="E35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B36" t="s">
         <v>202</v>
       </c>
       <c r="C36" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
       <c r="D36" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
       <c r="E36" t="b">
-        <v>0</v>
-      </c>
-      <c r="F36" s="28">
-        <v>45277</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B37" t="s">
         <v>202</v>
       </c>
       <c r="C37" t="s">
-        <v>279</v>
+        <v>403</v>
       </c>
       <c r="D37" t="s">
-        <v>256</v>
+        <v>226</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
       </c>
-      <c r="F37" s="28">
-        <v>45276</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B38" t="s">
         <v>202</v>
       </c>
       <c r="C38" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="D38" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
       </c>
-      <c r="F38">
-        <v>35.321100000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B39" t="s">
         <v>202</v>
       </c>
       <c r="C39" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D39" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
       </c>
-      <c r="F39">
-        <v>35.321100000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="28">
+        <v>45275</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B40" t="s">
         <v>202</v>
       </c>
       <c r="C40" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D40" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
       </c>
-      <c r="F40">
-        <v>-119.5808</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="28">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B41" t="s">
         <v>202</v>
       </c>
       <c r="C41" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="D41" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>-119.5808</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B42" t="s">
         <v>202</v>
       </c>
       <c r="C42" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D42" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="E42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B43" t="s">
         <v>202</v>
       </c>
       <c r="C43" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="D43" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
       </c>
-      <c r="F43" s="28">
-        <v>45275</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B44" t="s">
         <v>202</v>
       </c>
       <c r="C44" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="D44" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E44" t="b">
-        <v>0</v>
-      </c>
-      <c r="F44" s="28">
-        <v>45468</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B45" t="s">
         <v>202</v>
       </c>
       <c r="C45" t="s">
-        <v>246</v>
+        <v>405</v>
       </c>
       <c r="D45" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B46" t="s">
         <v>202</v>
       </c>
       <c r="C46" t="s">
-        <v>405</v>
+        <v>279</v>
       </c>
       <c r="D46" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
       </c>
-      <c r="F46" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="28">
+        <v>45276</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B47" t="s">
         <v>202</v>
       </c>
       <c r="C47" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="D47" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
       </c>
-      <c r="F47">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="28">
+        <v>45277</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B48" t="s">
         <v>202</v>
       </c>
       <c r="C48" t="s">
-        <v>267</v>
+        <v>401</v>
       </c>
       <c r="D48" t="s">
-        <v>277</v>
+        <v>218</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
       </c>
-      <c r="F48" s="28">
-        <v>85</v>
+      <c r="F48" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:F48">
-    <sortCondition ref="A1:A1048576"/>
-    <sortCondition ref="B1:B1048576"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:F48">
+    <sortCondition ref="C13:C48"/>
+    <sortCondition ref="D13:D48"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9644,29 +9644,29 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.87890625" customWidth="1"/>
+    <col min="5" max="5" width="13.703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5859375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.29296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.29296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.29296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" s="21" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="21" t="s">
         <v>418</v>
       </c>
       <c r="C2" s="22"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="6" spans="2:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="86" x14ac:dyDescent="0.5">
       <c r="B6" s="78" t="s">
         <v>406</v>
       </c>
@@ -9704,7 +9704,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B7" s="80"/>
       <c r="C7" s="80"/>
       <c r="D7" s="80"/>
@@ -9718,7 +9718,7 @@
       <c r="L7" s="80"/>
       <c r="M7" s="80"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B8" s="80"/>
       <c r="C8" s="80"/>
       <c r="D8" s="80"/>
@@ -9732,7 +9732,7 @@
       <c r="L8" s="80"/>
       <c r="M8" s="80"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B9" s="80"/>
       <c r="C9" s="80"/>
       <c r="D9" s="80"/>
@@ -9746,7 +9746,7 @@
       <c r="L9" s="80"/>
       <c r="M9" s="80"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B10" s="80"/>
       <c r="C10" s="80"/>
       <c r="D10" s="80"/>
@@ -9760,7 +9760,7 @@
       <c r="L10" s="80"/>
       <c r="M10" s="80"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B11" s="80"/>
       <c r="C11" s="80"/>
       <c r="D11" s="80"/>
@@ -9774,7 +9774,7 @@
       <c r="L11" s="80"/>
       <c r="M11" s="80"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B12" s="80"/>
       <c r="C12" s="80"/>
       <c r="D12" s="80"/>
@@ -9788,7 +9788,7 @@
       <c r="L12" s="80"/>
       <c r="M12" s="80"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B13" s="80"/>
       <c r="C13" s="80"/>
       <c r="D13" s="80"/>
@@ -9802,7 +9802,7 @@
       <c r="L13" s="80"/>
       <c r="M13" s="80"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B14" s="80"/>
       <c r="C14" s="80"/>
       <c r="D14" s="80"/>
@@ -9816,7 +9816,7 @@
       <c r="L14" s="80"/>
       <c r="M14" s="80"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B15" s="80"/>
       <c r="C15" s="80"/>
       <c r="D15" s="80"/>
@@ -9830,7 +9830,7 @@
       <c r="L15" s="80"/>
       <c r="M15" s="80"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B16" s="80"/>
       <c r="C16" s="80"/>
       <c r="D16" s="80"/>
@@ -9844,7 +9844,7 @@
       <c r="L16" s="80"/>
       <c r="M16" s="80"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B17" s="80"/>
       <c r="C17" s="80"/>
       <c r="D17" s="80"/>
@@ -9858,7 +9858,7 @@
       <c r="L17" s="80"/>
       <c r="M17" s="80"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B18" s="80"/>
       <c r="C18" s="80"/>
       <c r="D18" s="80"/>
@@ -9872,7 +9872,7 @@
       <c r="L18" s="80"/>
       <c r="M18" s="80"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B19" s="80"/>
       <c r="C19" s="80"/>
       <c r="D19" s="80"/>
@@ -9886,7 +9886,7 @@
       <c r="L19" s="80"/>
       <c r="M19" s="80"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B20" s="80"/>
       <c r="C20" s="80"/>
       <c r="D20" s="80"/>
@@ -9900,7 +9900,7 @@
       <c r="L20" s="80"/>
       <c r="M20" s="80"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B21" s="80"/>
       <c r="C21" s="80"/>
       <c r="D21" s="80"/>
@@ -9914,7 +9914,7 @@
       <c r="L21" s="80"/>
       <c r="M21" s="80"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B22" s="80"/>
       <c r="C22" s="80"/>
       <c r="D22" s="80"/>
@@ -9928,7 +9928,7 @@
       <c r="L22" s="80"/>
       <c r="M22" s="80"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B23" s="80"/>
       <c r="C23" s="80"/>
       <c r="D23" s="80"/>
@@ -9942,7 +9942,7 @@
       <c r="L23" s="80"/>
       <c r="M23" s="80"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B24" s="80"/>
       <c r="C24" s="80"/>
       <c r="D24" s="80"/>
@@ -9956,7 +9956,7 @@
       <c r="L24" s="80"/>
       <c r="M24" s="80"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B25" s="80"/>
       <c r="C25" s="80"/>
       <c r="D25" s="80"/>
@@ -9970,7 +9970,7 @@
       <c r="L25" s="80"/>
       <c r="M25" s="80"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.5">
       <c r="B26" s="80"/>
       <c r="C26" s="80"/>
       <c r="D26" s="80"/>
@@ -10225,15 +10225,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
@@ -10242,6 +10233,15 @@
     <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10264,14 +10264,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -10282,6 +10274,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{9de5aaee-7788-40b1-a438-c0ccc98c87cc}" enabled="0" method="" siteId="{9de5aaee-7788-40b1-a438-c0ccc98c87cc}" removed="1"/>

</xml_diff>